<commit_message>
cierre 23 de agosto
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14745" windowHeight="10725" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 1 " sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="76">
   <si>
     <t xml:space="preserve">ABASTO 4 CARNES </t>
   </si>
@@ -507,6 +507,9 @@
       </rPr>
       <t xml:space="preserve">        2 0 2 1</t>
     </r>
+  </si>
+  <si>
+    <t>MOSTRADOR MENUDEO</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1773,6 +1776,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2632,13 +2638,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>152402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2646,7 +2652,7 @@
         <xdr:cNvPr id="2" name="1 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2685,13 +2691,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>561977</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>123829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2699,7 +2705,7 @@
         <xdr:cNvPr id="3" name="2 Conector recto de flecha">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2757,7 +2763,7 @@
         <xdr:cNvPr id="2" name="Cerrar llave 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3122,25 +3128,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -5440,12 +5446,12 @@
       <c r="B89" s="36"/>
       <c r="C89" s="36"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="220">
+      <c r="E89" s="221">
         <f>E85-G85</f>
         <v>0</v>
       </c>
-      <c r="F89" s="221"/>
-      <c r="G89" s="222"/>
+      <c r="F89" s="222"/>
+      <c r="G89" s="223"/>
       <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5461,11 +5467,11 @@
       <c r="B91" s="36"/>
       <c r="C91" s="36"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="223" t="s">
+      <c r="E91" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F91" s="223"/>
-      <c r="G91" s="223"/>
+      <c r="F91" s="224"/>
+      <c r="G91" s="224"/>
       <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -5587,8 +5593,8 @@
   </sheetPr>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5608,19 +5614,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="224" t="s">
+      <c r="C1" s="225" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
       <c r="F1" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="224" t="s">
+      <c r="J1" s="225" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
+      <c r="K1" s="226"/>
+      <c r="L1" s="226"/>
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50"/>
@@ -7814,10 +7820,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="226" t="s">
+      <c r="B1" s="227" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="227"/>
+      <c r="C1" s="228"/>
       <c r="D1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7837,10 +7843,10 @@
       <c r="F2" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="228" t="s">
+      <c r="G2" s="229" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="229"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="65">
@@ -8106,25 +8112,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -10497,12 +10503,12 @@
       <c r="B95" s="36"/>
       <c r="C95" s="36"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="220">
+      <c r="E95" s="221">
         <f>E91-G91</f>
         <v>0</v>
       </c>
-      <c r="F95" s="221"/>
-      <c r="G95" s="222"/>
+      <c r="F95" s="222"/>
+      <c r="G95" s="223"/>
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -10518,11 +10524,11 @@
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="223" t="s">
+      <c r="E97" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F97" s="223"/>
-      <c r="G97" s="223"/>
+      <c r="F97" s="224"/>
+      <c r="G97" s="224"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
@@ -10665,25 +10671,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -13840,12 +13846,12 @@
       <c r="B124" s="36"/>
       <c r="C124" s="36"/>
       <c r="D124" s="2"/>
-      <c r="E124" s="220">
+      <c r="E124" s="221">
         <f>E120-G120</f>
         <v>0</v>
       </c>
-      <c r="F124" s="221"/>
-      <c r="G124" s="222"/>
+      <c r="F124" s="222"/>
+      <c r="G124" s="223"/>
       <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -13861,11 +13867,11 @@
       <c r="B126" s="36"/>
       <c r="C126" s="36"/>
       <c r="D126" s="2"/>
-      <c r="E126" s="223" t="s">
+      <c r="E126" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F126" s="223"/>
-      <c r="G126" s="223"/>
+      <c r="F126" s="224"/>
+      <c r="G126" s="224"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -14006,25 +14012,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -16469,12 +16475,12 @@
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="220">
+      <c r="E97" s="221">
         <f>E93-G93</f>
         <v>0</v>
       </c>
-      <c r="F97" s="221"/>
-      <c r="G97" s="222"/>
+      <c r="F97" s="222"/>
+      <c r="G97" s="223"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -16490,11 +16496,11 @@
       <c r="B99" s="36"/>
       <c r="C99" s="36"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="223" t="s">
+      <c r="E99" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F99" s="223"/>
-      <c r="G99" s="223"/>
+      <c r="F99" s="224"/>
+      <c r="G99" s="224"/>
       <c r="I99" s="2"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -16643,25 +16649,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -19795,12 +19801,12 @@
       <c r="B125" s="165"/>
       <c r="C125" s="36"/>
       <c r="D125" s="2"/>
-      <c r="E125" s="220">
+      <c r="E125" s="221">
         <f>E121-G121</f>
         <v>0</v>
       </c>
-      <c r="F125" s="221"/>
-      <c r="G125" s="222"/>
+      <c r="F125" s="222"/>
+      <c r="G125" s="223"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -19816,11 +19822,11 @@
       <c r="B127" s="165"/>
       <c r="C127" s="36"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="223" t="s">
+      <c r="E127" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F127" s="223"/>
-      <c r="G127" s="223"/>
+      <c r="F127" s="224"/>
+      <c r="G127" s="224"/>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -19963,25 +19969,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -22075,12 +22081,12 @@
       <c r="B85" s="165"/>
       <c r="C85" s="36"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="220">
+      <c r="E85" s="221">
         <f>E81-G81</f>
         <v>0</v>
       </c>
-      <c r="F85" s="221"/>
-      <c r="G85" s="222"/>
+      <c r="F85" s="222"/>
+      <c r="G85" s="223"/>
       <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -22096,11 +22102,11 @@
       <c r="B87" s="165"/>
       <c r="C87" s="36"/>
       <c r="D87" s="2"/>
-      <c r="E87" s="223" t="s">
+      <c r="E87" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F87" s="223"/>
-      <c r="G87" s="223"/>
+      <c r="F87" s="224"/>
+      <c r="G87" s="224"/>
       <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -22222,8 +22228,8 @@
   </sheetPr>
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -22242,25 +22248,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -23271,11 +23277,11 @@
         <v>44397</v>
       </c>
       <c r="G41" s="27">
-        <v>4307</v>
+        <v>4304</v>
       </c>
       <c r="H41" s="16">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -23857,11 +23863,15 @@
       <c r="E63" s="20">
         <v>1713</v>
       </c>
-      <c r="F63" s="49"/>
-      <c r="G63" s="27"/>
+      <c r="F63" s="91">
+        <v>44417</v>
+      </c>
+      <c r="G63" s="92">
+        <v>1713</v>
+      </c>
       <c r="H63" s="28">
         <f t="shared" si="0"/>
-        <v>1713</v>
+        <v>0</v>
       </c>
       <c r="L63" s="62"/>
       <c r="M63" s="62"/>
@@ -24433,8 +24443,8 @@
       <c r="E83" s="20">
         <v>1966</v>
       </c>
-      <c r="F83" s="49"/>
-      <c r="G83" s="27"/>
+      <c r="F83" s="91"/>
+      <c r="G83" s="92"/>
       <c r="H83" s="28">
         <f t="shared" si="0"/>
         <v>1966</v>
@@ -24455,11 +24465,15 @@
       <c r="E84" s="20">
         <v>4046</v>
       </c>
-      <c r="F84" s="49"/>
-      <c r="G84" s="27"/>
+      <c r="F84" s="91">
+        <v>44419</v>
+      </c>
+      <c r="G84" s="92">
+        <v>4046</v>
+      </c>
       <c r="H84" s="28">
         <f t="shared" si="0"/>
-        <v>4046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -24711,11 +24725,15 @@
       <c r="E94" s="27">
         <v>3504</v>
       </c>
-      <c r="F94" s="214"/>
-      <c r="G94" s="27"/>
+      <c r="F94" s="216">
+        <v>44414</v>
+      </c>
+      <c r="G94" s="92">
+        <v>3504</v>
+      </c>
       <c r="H94" s="28">
         <f t="shared" si="0"/>
-        <v>3504</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -24785,11 +24803,15 @@
       <c r="E97" s="27">
         <v>4478</v>
       </c>
-      <c r="F97" s="214"/>
-      <c r="G97" s="27"/>
+      <c r="F97" s="216">
+        <v>44423</v>
+      </c>
+      <c r="G97" s="92">
+        <v>4478</v>
+      </c>
       <c r="H97" s="28">
         <f t="shared" si="0"/>
-        <v>4478</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -24859,11 +24881,15 @@
       <c r="E100" s="27">
         <v>135</v>
       </c>
-      <c r="F100" s="214"/>
-      <c r="G100" s="27"/>
+      <c r="F100" s="216">
+        <v>44419</v>
+      </c>
+      <c r="G100" s="92">
+        <v>135</v>
+      </c>
       <c r="H100" s="28">
         <f t="shared" si="0"/>
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -24881,11 +24907,15 @@
       <c r="E101" s="27">
         <v>12505</v>
       </c>
-      <c r="F101" s="214"/>
-      <c r="G101" s="27"/>
+      <c r="F101" s="216">
+        <v>44412</v>
+      </c>
+      <c r="G101" s="92">
+        <v>12505</v>
+      </c>
       <c r="H101" s="28">
         <f t="shared" si="0"/>
-        <v>12505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -24903,11 +24933,15 @@
       <c r="E102" s="27">
         <v>1434</v>
       </c>
-      <c r="F102" s="214"/>
-      <c r="G102" s="27"/>
+      <c r="F102" s="216">
+        <v>44413</v>
+      </c>
+      <c r="G102" s="92">
+        <v>1434</v>
+      </c>
       <c r="H102" s="28">
         <f t="shared" si="0"/>
-        <v>1434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -25015,11 +25049,11 @@
       <c r="F110" s="37"/>
       <c r="G110" s="37">
         <f>SUM(G4:G109)</f>
-        <v>1120514</v>
+        <v>1148326</v>
       </c>
       <c r="H110" s="38">
         <f>SUM(H4:H109)</f>
-        <v>29778</v>
+        <v>1966</v>
       </c>
       <c r="I110" s="2"/>
     </row>
@@ -25061,12 +25095,12 @@
       <c r="B114" s="165"/>
       <c r="C114" s="36"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="220">
+      <c r="E114" s="221">
         <f>E110-G110</f>
-        <v>29778</v>
-      </c>
-      <c r="F114" s="221"/>
-      <c r="G114" s="222"/>
+        <v>1966</v>
+      </c>
+      <c r="F114" s="222"/>
+      <c r="G114" s="223"/>
       <c r="I114" s="2"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -25082,11 +25116,11 @@
       <c r="B116" s="165"/>
       <c r="C116" s="36"/>
       <c r="D116" s="2"/>
-      <c r="E116" s="223" t="s">
+      <c r="E116" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F116" s="223"/>
-      <c r="G116" s="223"/>
+      <c r="F116" s="224"/>
+      <c r="G116" s="224"/>
       <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -25206,10 +25240,13 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:Q127"/>
+  <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D91" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25228,25 +25265,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="217" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="217"/>
-      <c r="D1" s="217"/>
-      <c r="E1" s="217"/>
-      <c r="F1" s="217"/>
-      <c r="G1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="219"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
+      <c r="B2" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -25277,912 +25314,1482 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="11">
+        <v>44412</v>
+      </c>
       <c r="B4" s="12">
         <v>2293</v>
       </c>
       <c r="C4" s="13"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="19">
+        <v>9594</v>
+      </c>
+      <c r="F4" s="47">
+        <v>44421</v>
+      </c>
+      <c r="G4" s="25">
+        <v>9594</v>
+      </c>
       <c r="H4" s="16">
-        <f t="shared" ref="H4:H109" si="0">E4-G4</f>
+        <f t="shared" ref="H4:H126" si="0">E4-G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="11">
+        <v>44412</v>
+      </c>
       <c r="B5" s="12">
         <f>B4+1</f>
         <v>2294</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1478</v>
+      </c>
+      <c r="F5" s="49">
+        <v>44415</v>
+      </c>
+      <c r="G5" s="27">
+        <v>1478</v>
+      </c>
       <c r="H5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="11">
+        <v>44413</v>
+      </c>
       <c r="B6" s="12">
         <f t="shared" ref="B6:B69" si="1">B5+1</f>
         <v>2295</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="27"/>
+      <c r="D6" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="20">
+        <v>457</v>
+      </c>
+      <c r="F6" s="49">
+        <v>44419</v>
+      </c>
+      <c r="G6" s="27">
+        <v>457</v>
+      </c>
       <c r="H6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="18">
+        <v>44413</v>
+      </c>
       <c r="B7" s="12">
         <f t="shared" si="1"/>
         <v>2296</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="27"/>
+      <c r="D7" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="20">
+        <v>1577</v>
+      </c>
+      <c r="F7" s="49">
+        <v>44418</v>
+      </c>
+      <c r="G7" s="27">
+        <v>1577</v>
+      </c>
       <c r="H7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="11">
+        <v>44413</v>
+      </c>
       <c r="B8" s="12">
         <f t="shared" si="1"/>
         <v>2297</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="20">
+        <v>2193</v>
+      </c>
+      <c r="F8" s="49">
+        <v>44418</v>
+      </c>
+      <c r="G8" s="27">
+        <v>2193</v>
+      </c>
       <c r="H8" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="11">
+        <v>44413</v>
+      </c>
       <c r="B9" s="12">
         <f t="shared" si="1"/>
         <v>2298</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="20">
+        <v>1756</v>
+      </c>
+      <c r="F9" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1756</v>
+      </c>
       <c r="H9" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="11">
+        <v>44414</v>
+      </c>
       <c r="B10" s="12">
         <f t="shared" si="1"/>
         <v>2299</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="27"/>
+      <c r="D10" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="20">
+        <v>47</v>
+      </c>
+      <c r="F10" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G10" s="27">
+        <v>47</v>
+      </c>
       <c r="H10" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="11">
+        <v>44414</v>
+      </c>
       <c r="B11" s="12">
         <f t="shared" si="1"/>
         <v>2300</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="27"/>
+      <c r="D11" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="20">
+        <v>503</v>
+      </c>
+      <c r="F11" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G11" s="27">
+        <v>503</v>
+      </c>
       <c r="H11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="11">
+        <v>44414</v>
+      </c>
       <c r="B12" s="12">
         <f t="shared" si="1"/>
         <v>2301</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="20">
+        <v>110</v>
+      </c>
+      <c r="F12" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G12" s="27">
+        <v>110</v>
+      </c>
       <c r="H12" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11">
+        <v>44414</v>
+      </c>
       <c r="B13" s="12">
         <f t="shared" si="1"/>
         <v>2302</v>
       </c>
       <c r="C13" s="48"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="27"/>
+      <c r="D13" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="20">
+        <v>86</v>
+      </c>
+      <c r="F13" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G13" s="27">
+        <v>86</v>
+      </c>
       <c r="H13" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="11">
+        <v>44414</v>
+      </c>
       <c r="B14" s="12">
         <f t="shared" si="1"/>
         <v>2303</v>
       </c>
       <c r="C14" s="21"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="27"/>
+      <c r="D14" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="20">
+        <v>709</v>
+      </c>
+      <c r="F14" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G14" s="27">
+        <v>709</v>
+      </c>
       <c r="H14" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="11">
+        <v>44414</v>
+      </c>
       <c r="B15" s="12">
         <f t="shared" si="1"/>
         <v>2304</v>
       </c>
       <c r="C15" s="48"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="27"/>
+      <c r="D15" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="20">
+        <v>555</v>
+      </c>
+      <c r="F15" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G15" s="27">
+        <v>555</v>
+      </c>
       <c r="H15" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="11">
+        <v>44414</v>
+      </c>
       <c r="B16" s="12">
         <f t="shared" si="1"/>
         <v>2305</v>
       </c>
       <c r="C16" s="21"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="27"/>
+      <c r="D16" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="20">
+        <v>85</v>
+      </c>
+      <c r="F16" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G16" s="27">
+        <v>85</v>
+      </c>
       <c r="H16" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="11">
+        <v>44414</v>
+      </c>
       <c r="B17" s="12">
         <f t="shared" si="1"/>
         <v>2306</v>
       </c>
       <c r="C17" s="48"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="27"/>
+      <c r="D17" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="20">
+        <v>152</v>
+      </c>
+      <c r="F17" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G17" s="27">
+        <v>152</v>
+      </c>
       <c r="H17" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="11">
+        <v>44414</v>
+      </c>
       <c r="B18" s="12">
         <f t="shared" si="1"/>
         <v>2307</v>
       </c>
       <c r="C18" s="21"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="27"/>
+      <c r="D18" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="20">
+        <v>264</v>
+      </c>
+      <c r="F18" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G18" s="27">
+        <v>264</v>
+      </c>
       <c r="H18" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="11">
+        <v>44414</v>
+      </c>
       <c r="B19" s="12">
         <f t="shared" si="1"/>
         <v>2308</v>
       </c>
       <c r="C19" s="48"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="27"/>
+      <c r="D19" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="20">
+        <v>136</v>
+      </c>
+      <c r="F19" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G19" s="27">
+        <v>136</v>
+      </c>
       <c r="H19" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="11">
+        <v>44414</v>
+      </c>
       <c r="B20" s="12">
         <f t="shared" si="1"/>
         <v>2309</v>
       </c>
       <c r="C20" s="21"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="27"/>
+      <c r="D20" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="20">
+        <v>1300</v>
+      </c>
+      <c r="F20" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G20" s="27">
+        <v>1300</v>
+      </c>
       <c r="H20" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="11">
+        <v>44414</v>
+      </c>
       <c r="B21" s="12">
         <f t="shared" si="1"/>
         <v>2310</v>
       </c>
       <c r="C21" s="21"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="27"/>
+      <c r="D21" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="20">
+        <v>50</v>
+      </c>
+      <c r="F21" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G21" s="27">
+        <v>50</v>
+      </c>
       <c r="H21" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="11">
+        <v>44414</v>
+      </c>
       <c r="B22" s="12">
         <f t="shared" si="1"/>
         <v>2311</v>
       </c>
       <c r="C22" s="21"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="27"/>
+      <c r="D22" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="20">
+        <v>213</v>
+      </c>
+      <c r="F22" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G22" s="27">
+        <v>213</v>
+      </c>
       <c r="H22" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="11">
+        <v>44414</v>
+      </c>
       <c r="B23" s="12">
         <f t="shared" si="1"/>
         <v>2312</v>
       </c>
       <c r="C23" s="21"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="27"/>
+      <c r="D23" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="20">
+        <v>37</v>
+      </c>
+      <c r="F23" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G23" s="27">
+        <v>37</v>
+      </c>
       <c r="H23" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="A24" s="11">
+        <v>44414</v>
+      </c>
       <c r="B24" s="12">
         <f t="shared" si="1"/>
         <v>2313</v>
       </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="27"/>
+      <c r="D24" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="20">
+        <v>124</v>
+      </c>
+      <c r="F24" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G24" s="27">
+        <v>124</v>
+      </c>
       <c r="H24" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="A25" s="11">
+        <v>44414</v>
+      </c>
       <c r="B25" s="12">
         <f t="shared" si="1"/>
         <v>2314</v>
       </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="27"/>
+      <c r="D25" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="20">
+        <v>59</v>
+      </c>
+      <c r="F25" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G25" s="27">
+        <v>59</v>
+      </c>
       <c r="H25" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="A26" s="11">
+        <v>44414</v>
+      </c>
       <c r="B26" s="12">
         <f t="shared" si="1"/>
         <v>2315</v>
       </c>
       <c r="C26" s="21"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="27"/>
+      <c r="D26" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="20">
+        <v>23</v>
+      </c>
+      <c r="F26" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G26" s="27">
+        <v>23</v>
+      </c>
       <c r="H26" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="11">
+        <v>44414</v>
+      </c>
       <c r="B27" s="12">
         <f t="shared" si="1"/>
         <v>2316</v>
       </c>
       <c r="C27" s="21"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="27"/>
+      <c r="D27" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="20">
+        <v>268</v>
+      </c>
+      <c r="F27" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G27" s="27">
+        <v>268</v>
+      </c>
       <c r="H27" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="11">
+        <v>44414</v>
+      </c>
       <c r="B28" s="12">
         <f t="shared" si="1"/>
         <v>2317</v>
       </c>
       <c r="C28" s="21"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="27"/>
+      <c r="D28" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="20">
+        <v>232</v>
+      </c>
+      <c r="F28" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G28" s="27">
+        <v>232</v>
+      </c>
       <c r="H28" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+      <c r="A29" s="11">
+        <v>44414</v>
+      </c>
       <c r="B29" s="12">
         <f t="shared" si="1"/>
         <v>2318</v>
       </c>
       <c r="C29" s="21"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="27"/>
+      <c r="D29" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="20">
+        <v>45</v>
+      </c>
+      <c r="F29" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G29" s="27">
+        <v>45</v>
+      </c>
       <c r="H29" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="A30" s="11">
+        <v>44414</v>
+      </c>
       <c r="B30" s="12">
         <f t="shared" si="1"/>
         <v>2319</v>
       </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="27"/>
+      <c r="D30" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="20">
+        <v>546</v>
+      </c>
+      <c r="F30" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G30" s="27">
+        <v>546</v>
+      </c>
       <c r="H30" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="11">
+        <v>44414</v>
+      </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
         <v>2320</v>
       </c>
       <c r="C31" s="21"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="27"/>
+      <c r="D31" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="20">
+        <v>50</v>
+      </c>
+      <c r="F31" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G31" s="27">
+        <v>50</v>
+      </c>
       <c r="H31" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="11">
+        <v>44414</v>
+      </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
         <v>2321</v>
       </c>
       <c r="C32" s="21"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="27"/>
+      <c r="D32" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="20">
+        <v>186</v>
+      </c>
+      <c r="F32" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G32" s="27">
+        <v>186</v>
+      </c>
       <c r="H32" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="11">
+        <v>44414</v>
+      </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
         <v>2322</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="27"/>
+      <c r="D33" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="20">
+        <v>67</v>
+      </c>
+      <c r="F33" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G33" s="27">
+        <v>67</v>
+      </c>
       <c r="H33" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="11">
+        <v>44414</v>
+      </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
         <v>2323</v>
       </c>
       <c r="C34" s="22"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="27"/>
+      <c r="D34" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="20">
+        <v>163</v>
+      </c>
+      <c r="F34" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G34" s="27">
+        <v>163</v>
+      </c>
       <c r="H34" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="11">
+        <v>44414</v>
+      </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
         <v>2324</v>
       </c>
       <c r="C35" s="23"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="27"/>
+      <c r="D35" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="20">
+        <v>80</v>
+      </c>
+      <c r="F35" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G35" s="27">
+        <v>80</v>
+      </c>
       <c r="H35" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="11">
+        <v>44414</v>
+      </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
         <v>2325</v>
       </c>
       <c r="C36" s="21"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="27"/>
+      <c r="D36" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="20">
+        <v>167</v>
+      </c>
+      <c r="F36" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G36" s="27">
+        <v>167</v>
+      </c>
       <c r="H36" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="11">
+        <v>44414</v>
+      </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
         <v>2326</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="27"/>
+      <c r="D37" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="20">
+        <v>202</v>
+      </c>
+      <c r="F37" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G37" s="27">
+        <v>202</v>
+      </c>
       <c r="H37" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="11">
+        <v>44414</v>
+      </c>
       <c r="B38" s="12">
         <f t="shared" si="1"/>
         <v>2327</v>
       </c>
       <c r="C38" s="21"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="27"/>
+      <c r="D38" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="20">
+        <v>157</v>
+      </c>
+      <c r="F38" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G38" s="27">
+        <v>157</v>
+      </c>
       <c r="H38" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="11">
+        <v>44414</v>
+      </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
         <v>2328</v>
       </c>
       <c r="C39" s="21"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="27"/>
+      <c r="D39" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="20">
+        <v>48</v>
+      </c>
+      <c r="F39" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G39" s="27">
+        <v>48</v>
+      </c>
       <c r="H39" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="11">
+        <v>44414</v>
+      </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
         <v>2329</v>
       </c>
       <c r="C40" s="21"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="27"/>
+      <c r="D40" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="20">
+        <v>53</v>
+      </c>
+      <c r="F40" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G40" s="27">
+        <v>53</v>
+      </c>
       <c r="H40" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="11">
+        <v>44414</v>
+      </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
         <v>2330</v>
       </c>
       <c r="C41" s="21"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="27"/>
+      <c r="D41" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="20">
+        <v>206</v>
+      </c>
+      <c r="F41" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G41" s="27">
+        <v>206</v>
+      </c>
       <c r="H41" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="11">
+        <v>44414</v>
+      </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
         <v>2331</v>
       </c>
       <c r="C42" s="21"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="27"/>
+      <c r="D42" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="20">
+        <v>218</v>
+      </c>
+      <c r="F42" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G42" s="27">
+        <v>218</v>
+      </c>
       <c r="H42" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="11">
+        <v>44414</v>
+      </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
         <v>2332</v>
       </c>
       <c r="C43" s="21"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="27"/>
+      <c r="D43" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="20">
+        <v>496</v>
+      </c>
+      <c r="F43" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G43" s="27">
+        <v>496</v>
+      </c>
       <c r="H43" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="11">
+        <v>44414</v>
+      </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
         <v>2333</v>
       </c>
       <c r="C44" s="21"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="27"/>
+      <c r="D44" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="20">
+        <v>98</v>
+      </c>
+      <c r="F44" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G44" s="27">
+        <v>98</v>
+      </c>
       <c r="H44" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+      <c r="A45" s="11">
+        <v>44414</v>
+      </c>
       <c r="B45" s="12">
         <f t="shared" si="1"/>
         <v>2334</v>
       </c>
       <c r="C45" s="21"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="27"/>
+      <c r="D45" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="20">
+        <v>213</v>
+      </c>
+      <c r="F45" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G45" s="27">
+        <v>213</v>
+      </c>
       <c r="H45" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+      <c r="A46" s="11">
+        <v>44414</v>
+      </c>
       <c r="B46" s="12">
         <f t="shared" si="1"/>
         <v>2335</v>
       </c>
       <c r="C46" s="21"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="27"/>
+      <c r="D46" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="20">
+        <v>174</v>
+      </c>
+      <c r="F46" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G46" s="27">
+        <v>174</v>
+      </c>
       <c r="H46" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+      <c r="A47" s="11">
+        <v>44414</v>
+      </c>
       <c r="B47" s="12">
         <f t="shared" si="1"/>
         <v>2336</v>
       </c>
       <c r="C47" s="21"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="27"/>
+      <c r="D47" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="20">
+        <v>125</v>
+      </c>
+      <c r="F47" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G47" s="27">
+        <v>125</v>
+      </c>
       <c r="H47" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
+      <c r="A48" s="11">
+        <v>44414</v>
+      </c>
       <c r="B48" s="12">
         <f t="shared" si="1"/>
         <v>2337</v>
       </c>
       <c r="C48" s="21"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="27"/>
+      <c r="D48" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="20">
+        <v>563</v>
+      </c>
+      <c r="F48" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G48" s="27">
+        <v>563</v>
+      </c>
       <c r="H48" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="11">
+        <v>44414</v>
+      </c>
       <c r="B49" s="12">
         <f t="shared" si="1"/>
         <v>2338</v>
       </c>
       <c r="C49" s="21"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="27"/>
+      <c r="D49" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" s="20">
+        <v>35</v>
+      </c>
+      <c r="F49" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G49" s="27">
+        <v>35</v>
+      </c>
       <c r="H49" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
+      <c r="A50" s="11">
+        <v>44414</v>
+      </c>
       <c r="B50" s="12">
         <f t="shared" si="1"/>
         <v>2339</v>
       </c>
       <c r="C50" s="21"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="27"/>
+      <c r="D50" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="20">
+        <v>253</v>
+      </c>
+      <c r="F50" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G50" s="27">
+        <v>253</v>
+      </c>
       <c r="H50" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="11">
+        <v>44414</v>
+      </c>
       <c r="B51" s="12">
         <f t="shared" si="1"/>
         <v>2340</v>
       </c>
       <c r="C51" s="21"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="27"/>
+      <c r="D51" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="20">
+        <v>81</v>
+      </c>
+      <c r="F51" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G51" s="27">
+        <v>81</v>
+      </c>
       <c r="H51" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="11">
+        <v>44414</v>
+      </c>
       <c r="B52" s="12">
         <f t="shared" si="1"/>
         <v>2341</v>
       </c>
       <c r="C52" s="21"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="27"/>
+      <c r="D52" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="20">
+        <v>127</v>
+      </c>
+      <c r="F52" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G52" s="27">
+        <v>127</v>
+      </c>
       <c r="H52" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="11">
+        <v>44414</v>
+      </c>
       <c r="B53" s="12">
         <f t="shared" si="1"/>
         <v>2342</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="27"/>
+      <c r="D53" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="20">
+        <v>107</v>
+      </c>
+      <c r="F53" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G53" s="27">
+        <v>107</v>
+      </c>
       <c r="H53" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+      <c r="A54" s="11">
+        <v>44414</v>
+      </c>
       <c r="B54" s="12">
         <f t="shared" si="1"/>
         <v>2343</v>
       </c>
       <c r="C54" s="21"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="27"/>
+      <c r="D54" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="20">
+        <v>48</v>
+      </c>
+      <c r="F54" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G54" s="27">
+        <v>48</v>
+      </c>
       <c r="H54" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
+      <c r="A55" s="11">
+        <v>44414</v>
+      </c>
       <c r="B55" s="12">
         <f t="shared" si="1"/>
         <v>2344</v>
       </c>
       <c r="C55" s="21"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="27"/>
+      <c r="D55" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="20">
+        <v>132</v>
+      </c>
+      <c r="F55" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G55" s="27">
+        <v>132</v>
+      </c>
       <c r="H55" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
+      <c r="A56" s="11">
+        <v>44414</v>
+      </c>
       <c r="B56" s="12">
         <f t="shared" si="1"/>
         <v>2345</v>
       </c>
       <c r="C56" s="21"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="27"/>
+      <c r="D56" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="20">
+        <v>204</v>
+      </c>
+      <c r="F56" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G56" s="27">
+        <v>204</v>
+      </c>
       <c r="H56" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+      <c r="A57" s="11">
+        <v>44414</v>
+      </c>
       <c r="B57" s="12">
         <f t="shared" si="1"/>
         <v>2346</v>
       </c>
       <c r="C57" s="21"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="27"/>
+      <c r="D57" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E57" s="20">
+        <v>123</v>
+      </c>
+      <c r="F57" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G57" s="27">
+        <v>123</v>
+      </c>
       <c r="H57" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+      <c r="A58" s="11">
+        <v>44414</v>
+      </c>
       <c r="B58" s="12">
         <f t="shared" si="1"/>
         <v>2347</v>
       </c>
       <c r="C58" s="21"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="27"/>
+      <c r="D58" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58" s="20">
+        <v>266</v>
+      </c>
+      <c r="F58" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G58" s="27">
+        <v>266</v>
+      </c>
       <c r="H58" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+      <c r="A59" s="11">
+        <v>44414</v>
+      </c>
       <c r="B59" s="12">
         <f t="shared" si="1"/>
         <v>2348</v>
       </c>
       <c r="C59" s="21"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="27"/>
+      <c r="D59" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" s="20">
+        <v>46</v>
+      </c>
+      <c r="F59" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G59" s="27">
+        <v>46</v>
+      </c>
       <c r="H59" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
+      <c r="A60" s="11">
+        <v>44414</v>
+      </c>
       <c r="B60" s="12">
         <f t="shared" si="1"/>
         <v>2349</v>
       </c>
       <c r="C60" s="21"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="27"/>
+      <c r="D60" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" s="20">
+        <v>544</v>
+      </c>
+      <c r="F60" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G60" s="27">
+        <v>544</v>
+      </c>
       <c r="H60" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26195,16 +26802,26 @@
       <c r="Q60" s="62"/>
     </row>
     <row r="61" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
+      <c r="A61" s="11">
+        <v>44414</v>
+      </c>
       <c r="B61" s="12">
         <f t="shared" si="1"/>
         <v>2350</v>
       </c>
       <c r="C61" s="21"/>
-      <c r="D61" s="43"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="27"/>
+      <c r="D61" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E61" s="20">
+        <v>176</v>
+      </c>
+      <c r="F61" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G61" s="27">
+        <v>176</v>
+      </c>
       <c r="H61" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26217,16 +26834,26 @@
       <c r="Q61" s="62"/>
     </row>
     <row r="62" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
+      <c r="A62" s="11">
+        <v>44414</v>
+      </c>
       <c r="B62" s="12">
         <f t="shared" si="1"/>
         <v>2351</v>
       </c>
       <c r="C62" s="21"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="27"/>
+      <c r="D62" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E62" s="20">
+        <v>209</v>
+      </c>
+      <c r="F62" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G62" s="27">
+        <v>209</v>
+      </c>
       <c r="H62" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26239,16 +26866,26 @@
       <c r="Q62" s="62"/>
     </row>
     <row r="63" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
+      <c r="A63" s="11">
+        <v>44414</v>
+      </c>
       <c r="B63" s="12">
         <f t="shared" si="1"/>
         <v>2352</v>
       </c>
       <c r="C63" s="21"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="27"/>
+      <c r="D63" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="20">
+        <v>133</v>
+      </c>
+      <c r="F63" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G63" s="27">
+        <v>133</v>
+      </c>
       <c r="H63" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26261,16 +26898,26 @@
       <c r="Q63" s="62"/>
     </row>
     <row r="64" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
+      <c r="A64" s="11">
+        <v>44414</v>
+      </c>
       <c r="B64" s="12">
         <f t="shared" si="1"/>
         <v>2353</v>
       </c>
       <c r="C64" s="21"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="27"/>
+      <c r="D64" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" s="20">
+        <v>201</v>
+      </c>
+      <c r="F64" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G64" s="27">
+        <v>201</v>
+      </c>
       <c r="H64" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26283,16 +26930,26 @@
       <c r="Q64" s="150"/>
     </row>
     <row r="65" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
+      <c r="A65" s="11">
+        <v>44414</v>
+      </c>
       <c r="B65" s="12">
         <f t="shared" si="1"/>
         <v>2354</v>
       </c>
       <c r="C65" s="21"/>
-      <c r="D65" s="43"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="27"/>
+      <c r="D65" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="20">
+        <v>6054</v>
+      </c>
+      <c r="F65" s="49">
+        <v>44414</v>
+      </c>
+      <c r="G65" s="27">
+        <v>6054</v>
+      </c>
       <c r="H65" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26305,16 +26962,26 @@
       <c r="Q65" s="150"/>
     </row>
     <row r="66" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
+      <c r="A66" s="11">
+        <v>44414</v>
+      </c>
       <c r="B66" s="12">
         <f t="shared" si="1"/>
         <v>2355</v>
       </c>
       <c r="C66" s="21"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="27"/>
+      <c r="D66" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" s="20">
+        <v>110</v>
+      </c>
+      <c r="F66" s="49">
+        <v>44419</v>
+      </c>
+      <c r="G66" s="27">
+        <v>110</v>
+      </c>
       <c r="H66" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26327,16 +26994,26 @@
       <c r="Q66" s="150"/>
     </row>
     <row r="67" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
+      <c r="A67" s="11">
+        <v>44414</v>
+      </c>
       <c r="B67" s="12">
         <f t="shared" si="1"/>
         <v>2356</v>
       </c>
       <c r="C67" s="21"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="27"/>
+      <c r="D67" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="20">
+        <v>8180</v>
+      </c>
+      <c r="F67" s="49">
+        <v>44415</v>
+      </c>
+      <c r="G67" s="27">
+        <v>8180</v>
+      </c>
       <c r="H67" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26349,16 +27026,26 @@
       <c r="Q67" s="150"/>
     </row>
     <row r="68" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
+      <c r="A68" s="18">
+        <v>44415</v>
+      </c>
       <c r="B68" s="12">
         <f t="shared" si="1"/>
         <v>2357</v>
       </c>
       <c r="C68" s="21"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="27"/>
+      <c r="D68" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="20">
+        <v>784</v>
+      </c>
+      <c r="F68" s="49">
+        <v>44419</v>
+      </c>
+      <c r="G68" s="27">
+        <v>784</v>
+      </c>
       <c r="H68" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26371,16 +27058,26 @@
       <c r="Q68" s="150"/>
     </row>
     <row r="69" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+      <c r="A69" s="18">
+        <v>44415</v>
+      </c>
       <c r="B69" s="12">
         <f t="shared" si="1"/>
         <v>2358</v>
       </c>
       <c r="C69" s="21"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="27"/>
+      <c r="D69" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="20">
+        <v>45334</v>
+      </c>
+      <c r="F69" s="49">
+        <v>44417</v>
+      </c>
+      <c r="G69" s="27">
+        <v>45334</v>
+      </c>
       <c r="H69" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26393,16 +27090,26 @@
       <c r="Q69" s="150"/>
     </row>
     <row r="70" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
+      <c r="A70" s="18">
+        <v>44415</v>
+      </c>
       <c r="B70" s="12">
-        <f t="shared" ref="B70:B102" si="2">B69+1</f>
+        <f t="shared" ref="B70:B126" si="2">B69+1</f>
         <v>2359</v>
       </c>
       <c r="C70" s="21"/>
-      <c r="D70" s="43"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="27"/>
+      <c r="D70" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="20">
+        <v>3816</v>
+      </c>
+      <c r="F70" s="49">
+        <v>44416</v>
+      </c>
+      <c r="G70" s="27">
+        <v>3816</v>
+      </c>
       <c r="H70" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26415,16 +27122,26 @@
       <c r="Q70" s="62"/>
     </row>
     <row r="71" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+      <c r="A71" s="18">
+        <v>44415</v>
+      </c>
       <c r="B71" s="12">
         <f t="shared" si="2"/>
         <v>2360</v>
       </c>
       <c r="C71" s="21"/>
-      <c r="D71" s="43"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="49"/>
-      <c r="G71" s="27"/>
+      <c r="D71" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="20">
+        <v>16643</v>
+      </c>
+      <c r="F71" s="49">
+        <v>44416</v>
+      </c>
+      <c r="G71" s="27">
+        <v>16643</v>
+      </c>
       <c r="H71" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26437,16 +27154,26 @@
       <c r="Q71" s="62"/>
     </row>
     <row r="72" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
+      <c r="A72" s="18">
+        <v>44416</v>
+      </c>
       <c r="B72" s="12">
         <f t="shared" si="2"/>
         <v>2361</v>
       </c>
       <c r="C72" s="21"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="27"/>
+      <c r="D72" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="20">
+        <v>1041</v>
+      </c>
+      <c r="F72" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G72" s="27">
+        <v>1041</v>
+      </c>
       <c r="H72" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -26459,470 +27186,724 @@
       <c r="Q72" s="62"/>
     </row>
     <row r="73" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="18"/>
+      <c r="A73" s="18">
+        <v>44416</v>
+      </c>
       <c r="B73" s="12">
         <f t="shared" si="2"/>
         <v>2362</v>
       </c>
       <c r="C73" s="21"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="49"/>
-      <c r="G73" s="27"/>
+      <c r="D73" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E73" s="20">
+        <v>47792</v>
+      </c>
+      <c r="F73" s="49">
+        <v>44418</v>
+      </c>
+      <c r="G73" s="27">
+        <v>47792</v>
+      </c>
       <c r="H73" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18"/>
+      <c r="A74" s="18">
+        <v>44416</v>
+      </c>
       <c r="B74" s="12">
         <f t="shared" si="2"/>
         <v>2363</v>
       </c>
       <c r="C74" s="21"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="27"/>
+      <c r="D74" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="20">
+        <v>1203</v>
+      </c>
+      <c r="F74" s="49">
+        <v>44417</v>
+      </c>
+      <c r="G74" s="27">
+        <v>1203</v>
+      </c>
       <c r="H74" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
+      <c r="A75" s="18">
+        <v>44417</v>
+      </c>
       <c r="B75" s="12">
         <f t="shared" si="2"/>
         <v>2364</v>
       </c>
       <c r="C75" s="170"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="20"/>
+      <c r="D75" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="20">
+        <v>1654</v>
+      </c>
       <c r="F75" s="49"/>
       <c r="G75" s="27"/>
       <c r="H75" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
+      <c r="A76" s="18">
+        <v>44417</v>
+      </c>
       <c r="B76" s="12">
         <f t="shared" si="2"/>
         <v>2365</v>
       </c>
       <c r="C76" s="170"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="27"/>
+      <c r="D76" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="20">
+        <v>1231</v>
+      </c>
+      <c r="F76" s="49">
+        <v>44418</v>
+      </c>
+      <c r="G76" s="27">
+        <v>1231</v>
+      </c>
       <c r="H76" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
+      <c r="A77" s="18">
+        <v>44418</v>
+      </c>
       <c r="B77" s="12">
         <f t="shared" si="2"/>
         <v>2366</v>
       </c>
       <c r="C77" s="170"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="49"/>
-      <c r="G77" s="27"/>
+      <c r="D77" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E77" s="20">
+        <v>7664</v>
+      </c>
+      <c r="F77" s="49">
+        <v>44419</v>
+      </c>
+      <c r="G77" s="27">
+        <v>7664</v>
+      </c>
       <c r="H77" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="18"/>
+      <c r="A78" s="18">
+        <v>44418</v>
+      </c>
       <c r="B78" s="12">
         <f t="shared" si="2"/>
         <v>2367</v>
       </c>
       <c r="C78" s="170"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="49"/>
-      <c r="G78" s="27"/>
+      <c r="D78" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E78" s="20">
+        <v>40103</v>
+      </c>
+      <c r="F78" s="49">
+        <v>44420</v>
+      </c>
+      <c r="G78" s="27">
+        <v>40103</v>
+      </c>
       <c r="H78" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
+      <c r="A79" s="18">
+        <v>44418</v>
+      </c>
       <c r="B79" s="12">
         <f t="shared" si="2"/>
         <v>2368</v>
       </c>
       <c r="C79" s="170"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="49"/>
-      <c r="G79" s="27"/>
+      <c r="D79" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="20">
+        <v>2939</v>
+      </c>
+      <c r="F79" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G79" s="27">
+        <v>2939</v>
+      </c>
       <c r="H79" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" s="18"/>
+      <c r="A80" s="18">
+        <v>44418</v>
+      </c>
       <c r="B80" s="12">
         <f t="shared" si="2"/>
         <v>2369</v>
       </c>
       <c r="C80" s="170"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="27"/>
+      <c r="D80" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="20">
+        <v>1205</v>
+      </c>
+      <c r="F80" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G80" s="27">
+        <v>1205</v>
+      </c>
       <c r="H80" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="18"/>
+      <c r="A81" s="18">
+        <v>44418</v>
+      </c>
       <c r="B81" s="12">
         <f t="shared" si="2"/>
         <v>2370</v>
       </c>
       <c r="C81" s="170"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="27"/>
+      <c r="D81" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E81" s="20">
+        <v>4633</v>
+      </c>
+      <c r="F81" s="49">
+        <v>44421</v>
+      </c>
+      <c r="G81" s="27">
+        <v>4633</v>
+      </c>
       <c r="H81" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="18"/>
+      <c r="A82" s="18">
+        <v>44418</v>
+      </c>
       <c r="B82" s="12">
         <f t="shared" si="2"/>
         <v>2371</v>
       </c>
       <c r="C82" s="170"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="27"/>
+      <c r="D82" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="20">
+        <v>1685</v>
+      </c>
+      <c r="F82" s="49">
+        <v>44419</v>
+      </c>
+      <c r="G82" s="27">
+        <v>1685</v>
+      </c>
       <c r="H82" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="18"/>
+      <c r="A83" s="18">
+        <v>44419</v>
+      </c>
       <c r="B83" s="12">
         <f t="shared" si="2"/>
         <v>2372</v>
       </c>
       <c r="C83" s="170"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="49"/>
-      <c r="G83" s="27"/>
+      <c r="D83" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" s="20">
+        <v>1807</v>
+      </c>
+      <c r="F83" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G83" s="27">
+        <v>1807</v>
+      </c>
       <c r="H83" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
+      <c r="A84" s="18">
+        <v>44420</v>
+      </c>
       <c r="B84" s="12">
         <f t="shared" si="2"/>
         <v>2373</v>
       </c>
       <c r="C84" s="170"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="27"/>
+      <c r="D84" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" s="20">
+        <v>7830</v>
+      </c>
+      <c r="F84" s="49">
+        <v>44425</v>
+      </c>
+      <c r="G84" s="27">
+        <v>7830</v>
+      </c>
       <c r="H84" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
+      <c r="A85" s="18">
+        <v>44420</v>
+      </c>
       <c r="B85" s="12">
         <f t="shared" si="2"/>
         <v>2374</v>
       </c>
       <c r="C85" s="170"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="27"/>
+      <c r="D85" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E85" s="20">
+        <v>40454</v>
+      </c>
+      <c r="F85" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G85" s="27">
+        <v>40454</v>
+      </c>
       <c r="H85" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
+      <c r="A86" s="18">
+        <v>44420</v>
+      </c>
       <c r="B86" s="12">
         <f t="shared" si="2"/>
         <v>2375</v>
       </c>
       <c r="C86" s="170"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="20"/>
+      <c r="D86" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" s="20">
+        <v>6222</v>
+      </c>
       <c r="F86" s="49"/>
       <c r="G86" s="27"/>
       <c r="H86" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6222</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
+      <c r="A87" s="18">
+        <v>44421</v>
+      </c>
       <c r="B87" s="12">
         <f t="shared" si="2"/>
         <v>2376</v>
       </c>
       <c r="C87" s="170"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="27"/>
+      <c r="D87" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E87" s="20">
+        <v>1159</v>
+      </c>
+      <c r="F87" s="49">
+        <v>44424</v>
+      </c>
+      <c r="G87" s="27">
+        <v>1159</v>
+      </c>
       <c r="H87" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="18"/>
+      <c r="A88" s="18">
+        <v>44421</v>
+      </c>
       <c r="B88" s="12">
         <f t="shared" si="2"/>
         <v>2377</v>
       </c>
       <c r="C88" s="170"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="49"/>
-      <c r="G88" s="27"/>
+      <c r="D88" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="20">
+        <v>1797</v>
+      </c>
+      <c r="F88" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G88" s="27">
+        <v>1797</v>
+      </c>
       <c r="H88" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="18"/>
+      <c r="A89" s="18">
+        <v>44421</v>
+      </c>
       <c r="B89" s="12">
         <f t="shared" si="2"/>
         <v>2378</v>
       </c>
       <c r="C89" s="170"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="49"/>
-      <c r="G89" s="27"/>
+      <c r="D89" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E89" s="20">
+        <v>8356</v>
+      </c>
+      <c r="F89" s="49">
+        <v>44422</v>
+      </c>
+      <c r="G89" s="27">
+        <v>8356</v>
+      </c>
       <c r="H89" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="157"/>
+      <c r="A90" s="157">
+        <v>44422</v>
+      </c>
       <c r="B90" s="12">
         <f t="shared" si="2"/>
         <v>2379</v>
       </c>
       <c r="C90" s="171"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="27"/>
-      <c r="F90" s="214"/>
-      <c r="G90" s="27"/>
+      <c r="D90" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E90" s="27">
+        <v>105</v>
+      </c>
+      <c r="F90" s="214">
+        <v>44424</v>
+      </c>
+      <c r="G90" s="27">
+        <v>105</v>
+      </c>
       <c r="H90" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="157"/>
+      <c r="A91" s="157">
+        <v>44422</v>
+      </c>
       <c r="B91" s="12">
         <f t="shared" si="2"/>
         <v>2380</v>
       </c>
       <c r="C91" s="213"/>
-      <c r="D91" s="45"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="214"/>
-      <c r="G91" s="27"/>
+      <c r="D91" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E91" s="27">
+        <v>41532</v>
+      </c>
+      <c r="F91" s="214">
+        <v>44423</v>
+      </c>
+      <c r="G91" s="27">
+        <v>41532</v>
+      </c>
       <c r="H91" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="157"/>
+      <c r="A92" s="157">
+        <v>44422</v>
+      </c>
       <c r="B92" s="12">
         <f t="shared" si="2"/>
         <v>2381</v>
       </c>
       <c r="C92" s="213"/>
-      <c r="D92" s="45"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="214"/>
-      <c r="G92" s="27"/>
+      <c r="D92" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="27">
+        <v>16284</v>
+      </c>
+      <c r="F92" s="214">
+        <v>44423</v>
+      </c>
+      <c r="G92" s="27">
+        <v>16284</v>
+      </c>
       <c r="H92" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="157"/>
+      <c r="A93" s="157">
+        <v>44423</v>
+      </c>
       <c r="B93" s="12">
         <f t="shared" si="2"/>
         <v>2382</v>
       </c>
       <c r="C93" s="213"/>
-      <c r="D93" s="45"/>
-      <c r="E93" s="27"/>
+      <c r="D93" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" s="27">
+        <v>4166</v>
+      </c>
       <c r="F93" s="214"/>
       <c r="G93" s="27"/>
       <c r="H93" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="157"/>
+      <c r="A94" s="157">
+        <v>44423</v>
+      </c>
       <c r="B94" s="12">
         <f t="shared" si="2"/>
         <v>2383</v>
       </c>
       <c r="C94" s="213"/>
-      <c r="D94" s="45"/>
-      <c r="E94" s="27"/>
+      <c r="D94" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" s="27">
+        <v>3536</v>
+      </c>
       <c r="F94" s="214"/>
       <c r="G94" s="27"/>
       <c r="H94" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="157"/>
+      <c r="A95" s="157">
+        <v>44423</v>
+      </c>
       <c r="B95" s="12">
         <f t="shared" si="2"/>
         <v>2384</v>
       </c>
       <c r="C95" s="213"/>
-      <c r="D95" s="45"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="214"/>
-      <c r="G95" s="27"/>
+      <c r="D95" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E95" s="27">
+        <v>3484</v>
+      </c>
+      <c r="F95" s="214">
+        <v>44424</v>
+      </c>
+      <c r="G95" s="27">
+        <v>3484</v>
+      </c>
       <c r="H95" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="157"/>
+      <c r="A96" s="157">
+        <v>44424</v>
+      </c>
       <c r="B96" s="12">
         <f t="shared" si="2"/>
         <v>2385</v>
       </c>
       <c r="C96" s="213"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="27"/>
+      <c r="D96" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E96" s="27">
+        <v>8452</v>
+      </c>
       <c r="F96" s="214"/>
       <c r="G96" s="27"/>
       <c r="H96" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="157"/>
+        <v>8452</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="157">
+        <v>44424</v>
+      </c>
       <c r="B97" s="12">
         <f t="shared" si="2"/>
         <v>2386</v>
       </c>
       <c r="C97" s="213"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="214"/>
-      <c r="G97" s="27"/>
+      <c r="D97" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97" s="27">
+        <v>8239</v>
+      </c>
+      <c r="F97" s="214">
+        <v>44425</v>
+      </c>
+      <c r="G97" s="27">
+        <v>8239</v>
+      </c>
       <c r="H97" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="157"/>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="157">
+        <v>44425</v>
+      </c>
       <c r="B98" s="12">
         <f t="shared" si="2"/>
         <v>2387</v>
       </c>
       <c r="C98" s="213"/>
-      <c r="D98" s="45"/>
-      <c r="E98" s="27"/>
+      <c r="D98" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E98" s="27">
+        <v>44459</v>
+      </c>
       <c r="F98" s="214"/>
       <c r="G98" s="27"/>
       <c r="H98" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="157"/>
+        <v>44459</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="157">
+        <v>44425</v>
+      </c>
       <c r="B99" s="12">
         <f t="shared" si="2"/>
         <v>2388</v>
       </c>
       <c r="C99" s="213"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="27"/>
+      <c r="D99" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E99" s="27">
+        <v>7831</v>
+      </c>
       <c r="F99" s="214"/>
       <c r="G99" s="27"/>
       <c r="H99" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="157"/>
+        <v>7831</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="157">
+        <v>44425</v>
+      </c>
       <c r="B100" s="12">
         <f t="shared" si="2"/>
         <v>2389</v>
       </c>
       <c r="C100" s="213"/>
-      <c r="D100" s="45"/>
-      <c r="E100" s="27"/>
+      <c r="D100" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" s="27">
+        <v>1005</v>
+      </c>
       <c r="F100" s="214"/>
       <c r="G100" s="27"/>
       <c r="H100" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="157"/>
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="157">
+        <v>44425</v>
+      </c>
       <c r="B101" s="12">
         <f t="shared" si="2"/>
         <v>2390</v>
       </c>
       <c r="C101" s="213"/>
-      <c r="D101" s="45"/>
-      <c r="E101" s="27"/>
+      <c r="D101" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E101" s="27">
+        <v>1085</v>
+      </c>
       <c r="F101" s="214"/>
       <c r="G101" s="27"/>
       <c r="H101" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="157"/>
       <c r="B102" s="12">
         <f t="shared" si="2"/>
@@ -26938,9 +27919,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="157"/>
-      <c r="B103" s="12"/>
+      <c r="B103" s="12">
+        <f t="shared" si="2"/>
+        <v>2392</v>
+      </c>
       <c r="C103" s="213"/>
       <c r="D103" s="45"/>
       <c r="E103" s="27"/>
@@ -26951,9 +27935,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="157"/>
-      <c r="B104" s="12"/>
+      <c r="B104" s="12">
+        <f t="shared" si="2"/>
+        <v>2393</v>
+      </c>
       <c r="C104" s="213"/>
       <c r="D104" s="45"/>
       <c r="E104" s="27"/>
@@ -26964,9 +27951,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="157"/>
-      <c r="B105" s="12"/>
+      <c r="B105" s="12">
+        <f t="shared" si="2"/>
+        <v>2394</v>
+      </c>
       <c r="C105" s="213"/>
       <c r="D105" s="45"/>
       <c r="E105" s="27"/>
@@ -26977,9 +27967,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="157"/>
-      <c r="B106" s="12"/>
+      <c r="B106" s="12">
+        <f t="shared" si="2"/>
+        <v>2395</v>
+      </c>
       <c r="C106" s="213"/>
       <c r="D106" s="45"/>
       <c r="E106" s="27"/>
@@ -26990,9 +27983,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="157"/>
-      <c r="B107" s="12"/>
+      <c r="B107" s="12">
+        <f t="shared" si="2"/>
+        <v>2396</v>
+      </c>
       <c r="C107" s="213"/>
       <c r="D107" s="45"/>
       <c r="E107" s="27"/>
@@ -27003,9 +27999,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="157"/>
-      <c r="B108" s="12"/>
+      <c r="B108" s="12">
+        <f t="shared" si="2"/>
+        <v>2397</v>
+      </c>
       <c r="C108" s="213"/>
       <c r="D108" s="45"/>
       <c r="E108" s="119"/>
@@ -27016,213 +28015,434 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="31"/>
-      <c r="B109" s="215"/>
-      <c r="C109" s="33"/>
-      <c r="D109" s="34"/>
-      <c r="E109" s="35">
-        <v>0</v>
-      </c>
-      <c r="F109" s="82"/>
-      <c r="G109" s="83"/>
-      <c r="H109" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="165"/>
-      <c r="C110" s="36"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="37">
-        <f>SUM(E4:E109)</f>
-        <v>0</v>
-      </c>
-      <c r="F110" s="37"/>
-      <c r="G110" s="37">
-        <f>SUM(G4:G109)</f>
-        <v>0</v>
-      </c>
-      <c r="H110" s="38">
-        <f>SUM(H4:H109)</f>
-        <v>0</v>
-      </c>
-      <c r="I110" s="2"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="165"/>
-      <c r="C111" s="36"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="39"/>
-      <c r="F111" s="86"/>
-      <c r="G111" s="87"/>
-      <c r="H111" s="40"/>
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B112" s="165"/>
-      <c r="C112" s="36"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="F112" s="86"/>
-      <c r="G112" s="88" t="s">
-        <v>9</v>
-      </c>
-      <c r="H112" s="40"/>
-      <c r="I112" s="2"/>
-    </row>
-    <row r="113" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="165"/>
-      <c r="C113" s="36"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="41"/>
-      <c r="F113" s="86"/>
-      <c r="G113" s="88"/>
-      <c r="H113" s="40"/>
-      <c r="I113" s="2"/>
-    </row>
-    <row r="114" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B114" s="165"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="220">
-        <f>E110-G110</f>
-        <v>0</v>
-      </c>
-      <c r="F114" s="221"/>
-      <c r="G114" s="222"/>
-      <c r="I114" s="2"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="165"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="39"/>
-      <c r="F115" s="86"/>
-      <c r="G115" s="87"/>
-      <c r="I115" s="2"/>
+    <row r="109" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="157"/>
+      <c r="B109" s="12">
+        <f t="shared" si="2"/>
+        <v>2398</v>
+      </c>
+      <c r="C109" s="213"/>
+      <c r="D109" s="45"/>
+      <c r="E109" s="119"/>
+      <c r="F109" s="172"/>
+      <c r="G109" s="119"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A110" s="157"/>
+      <c r="B110" s="12">
+        <f t="shared" si="2"/>
+        <v>2399</v>
+      </c>
+      <c r="C110" s="213"/>
+      <c r="D110" s="45"/>
+      <c r="E110" s="119"/>
+      <c r="F110" s="172"/>
+      <c r="G110" s="119"/>
+      <c r="H110" s="28"/>
+    </row>
+    <row r="111" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A111" s="157"/>
+      <c r="B111" s="12">
+        <f t="shared" si="2"/>
+        <v>2400</v>
+      </c>
+      <c r="C111" s="213"/>
+      <c r="D111" s="45"/>
+      <c r="E111" s="119"/>
+      <c r="F111" s="172"/>
+      <c r="G111" s="119"/>
+      <c r="H111" s="28"/>
+    </row>
+    <row r="112" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A112" s="157"/>
+      <c r="B112" s="12">
+        <f t="shared" si="2"/>
+        <v>2401</v>
+      </c>
+      <c r="C112" s="213"/>
+      <c r="D112" s="45"/>
+      <c r="E112" s="119"/>
+      <c r="F112" s="172"/>
+      <c r="G112" s="119"/>
+      <c r="H112" s="28"/>
+    </row>
+    <row r="113" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="157"/>
+      <c r="B113" s="12">
+        <f t="shared" si="2"/>
+        <v>2402</v>
+      </c>
+      <c r="C113" s="213"/>
+      <c r="D113" s="45"/>
+      <c r="E113" s="119"/>
+      <c r="F113" s="172"/>
+      <c r="G113" s="119"/>
+      <c r="H113" s="28"/>
+    </row>
+    <row r="114" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A114" s="157"/>
+      <c r="B114" s="12">
+        <f t="shared" si="2"/>
+        <v>2403</v>
+      </c>
+      <c r="C114" s="213"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="119"/>
+      <c r="F114" s="172"/>
+      <c r="G114" s="119"/>
+      <c r="H114" s="28"/>
+    </row>
+    <row r="115" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A115" s="157"/>
+      <c r="B115" s="12">
+        <f t="shared" si="2"/>
+        <v>2404</v>
+      </c>
+      <c r="C115" s="213"/>
+      <c r="D115" s="45"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="172"/>
+      <c r="G115" s="119"/>
+      <c r="H115" s="28"/>
     </row>
     <row r="116" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B116" s="165"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="223" t="s">
-        <v>10</v>
-      </c>
-      <c r="F116" s="223"/>
-      <c r="G116" s="223"/>
-      <c r="I116" s="2"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B117" s="165"/>
-      <c r="C117" s="36"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="39"/>
-      <c r="F117" s="86"/>
-      <c r="G117" s="87"/>
-      <c r="I117" s="2"/>
+      <c r="A116" s="157"/>
+      <c r="B116" s="12">
+        <f t="shared" si="2"/>
+        <v>2405</v>
+      </c>
+      <c r="C116" s="213"/>
+      <c r="D116" s="45"/>
+      <c r="E116" s="119"/>
+      <c r="F116" s="172"/>
+      <c r="G116" s="119"/>
+      <c r="H116" s="28"/>
+    </row>
+    <row r="117" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="157"/>
+      <c r="B117" s="12">
+        <f t="shared" si="2"/>
+        <v>2406</v>
+      </c>
+      <c r="C117" s="213"/>
+      <c r="D117" s="45"/>
+      <c r="E117" s="119"/>
+      <c r="F117" s="172"/>
+      <c r="G117" s="119"/>
+      <c r="H117" s="28"/>
     </row>
     <row r="118" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A118" s="157"/>
-      <c r="B118" s="164"/>
-      <c r="C118" s="159"/>
-      <c r="D118" s="160"/>
-      <c r="E118" s="161"/>
-      <c r="F118" s="162"/>
-      <c r="G118" s="161"/>
-      <c r="I118" s="2"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B119" s="165"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="86"/>
-      <c r="G119" s="87"/>
-      <c r="I119" s="2"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B120" s="165"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="39"/>
-      <c r="F120" s="86"/>
-      <c r="G120" s="87"/>
-      <c r="I120" s="2"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B121" s="165"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="39"/>
-      <c r="F121" s="86"/>
-      <c r="G121" s="87"/>
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B122" s="165"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="39"/>
-      <c r="F122" s="86"/>
-      <c r="G122" s="87"/>
-      <c r="I122" s="2"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B123" s="165"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="39"/>
-      <c r="F123" s="86"/>
-      <c r="G123" s="87"/>
-      <c r="I123" s="2"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B124" s="165"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="39"/>
-      <c r="F124" s="86"/>
-      <c r="G124" s="87"/>
-      <c r="I124" s="2"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="165"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="39"/>
-      <c r="F125" s="86"/>
-      <c r="G125" s="87"/>
-      <c r="I125" s="2"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B126" s="165"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="39"/>
-      <c r="F126" s="86"/>
-      <c r="G126" s="87"/>
+      <c r="B118" s="12">
+        <f t="shared" si="2"/>
+        <v>2407</v>
+      </c>
+      <c r="C118" s="213"/>
+      <c r="D118" s="45"/>
+      <c r="E118" s="119"/>
+      <c r="F118" s="172"/>
+      <c r="G118" s="119"/>
+      <c r="H118" s="28"/>
+    </row>
+    <row r="119" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A119" s="157"/>
+      <c r="B119" s="12">
+        <f t="shared" si="2"/>
+        <v>2408</v>
+      </c>
+      <c r="C119" s="213"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="119"/>
+      <c r="F119" s="172"/>
+      <c r="G119" s="119"/>
+      <c r="H119" s="28"/>
+    </row>
+    <row r="120" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A120" s="157"/>
+      <c r="B120" s="12">
+        <f t="shared" si="2"/>
+        <v>2409</v>
+      </c>
+      <c r="C120" s="213"/>
+      <c r="D120" s="45"/>
+      <c r="E120" s="119"/>
+      <c r="F120" s="172"/>
+      <c r="G120" s="119"/>
+      <c r="H120" s="28"/>
+    </row>
+    <row r="121" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A121" s="157"/>
+      <c r="B121" s="12">
+        <f t="shared" si="2"/>
+        <v>2410</v>
+      </c>
+      <c r="C121" s="213"/>
+      <c r="D121" s="45"/>
+      <c r="E121" s="119"/>
+      <c r="F121" s="172"/>
+      <c r="G121" s="119"/>
+      <c r="H121" s="28"/>
+    </row>
+    <row r="122" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A122" s="157"/>
+      <c r="B122" s="12">
+        <f t="shared" si="2"/>
+        <v>2411</v>
+      </c>
+      <c r="C122" s="213"/>
+      <c r="D122" s="45"/>
+      <c r="E122" s="119"/>
+      <c r="F122" s="172"/>
+      <c r="G122" s="119"/>
+      <c r="H122" s="28"/>
+    </row>
+    <row r="123" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A123" s="157"/>
+      <c r="B123" s="12">
+        <f t="shared" si="2"/>
+        <v>2412</v>
+      </c>
+      <c r="C123" s="213"/>
+      <c r="D123" s="45"/>
+      <c r="E123" s="119"/>
+      <c r="F123" s="172"/>
+      <c r="G123" s="119"/>
+      <c r="H123" s="28"/>
+    </row>
+    <row r="124" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A124" s="157"/>
+      <c r="B124" s="12">
+        <f t="shared" si="2"/>
+        <v>2413</v>
+      </c>
+      <c r="C124" s="213"/>
+      <c r="D124" s="45"/>
+      <c r="E124" s="119"/>
+      <c r="F124" s="172"/>
+      <c r="G124" s="119"/>
+      <c r="H124" s="28"/>
+    </row>
+    <row r="125" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="157"/>
+      <c r="B125" s="12">
+        <f t="shared" si="2"/>
+        <v>2414</v>
+      </c>
+      <c r="C125" s="213"/>
+      <c r="D125" s="45"/>
+      <c r="E125" s="119"/>
+      <c r="F125" s="172"/>
+      <c r="G125" s="119"/>
+      <c r="H125" s="28"/>
+    </row>
+    <row r="126" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="31"/>
+      <c r="B126" s="215"/>
+      <c r="C126" s="33"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="35">
+        <v>0</v>
+      </c>
+      <c r="F126" s="82"/>
+      <c r="G126" s="83"/>
+      <c r="H126" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B127" s="165"/>
       <c r="C127" s="36"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="39"/>
-      <c r="F127" s="86"/>
-      <c r="G127" s="87"/>
+      <c r="E127" s="37">
+        <f>SUM(E4:E126)</f>
+        <v>428424</v>
+      </c>
+      <c r="F127" s="37"/>
+      <c r="G127" s="37">
+        <f>SUM(G4:G126)</f>
+        <v>350014</v>
+      </c>
+      <c r="H127" s="38">
+        <f>SUM(H4:H126)</f>
+        <v>78410</v>
+      </c>
       <c r="I127" s="2"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="165"/>
+      <c r="C128" s="36"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="39"/>
+      <c r="F128" s="86"/>
+      <c r="G128" s="87"/>
+      <c r="H128" s="40"/>
+      <c r="I128" s="2"/>
+    </row>
+    <row r="129" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B129" s="165"/>
+      <c r="C129" s="36"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F129" s="86"/>
+      <c r="G129" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" s="40"/>
+      <c r="I129" s="2"/>
+    </row>
+    <row r="130" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="165"/>
+      <c r="C130" s="36"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="41"/>
+      <c r="F130" s="86"/>
+      <c r="G130" s="88"/>
+      <c r="H130" s="40"/>
+      <c r="I130" s="2"/>
+    </row>
+    <row r="131" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B131" s="165"/>
+      <c r="C131" s="36"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="221">
+        <f>E127-G127</f>
+        <v>78410</v>
+      </c>
+      <c r="F131" s="222"/>
+      <c r="G131" s="223"/>
+      <c r="I131" s="2"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="165"/>
+      <c r="C132" s="36"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="39"/>
+      <c r="F132" s="86"/>
+      <c r="G132" s="87"/>
+      <c r="I132" s="2"/>
+    </row>
+    <row r="133" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B133" s="165"/>
+      <c r="C133" s="36"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="224" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="224"/>
+      <c r="G133" s="224"/>
+      <c r="I133" s="2"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="165"/>
+      <c r="C134" s="36"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="39"/>
+      <c r="F134" s="86"/>
+      <c r="G134" s="87"/>
+      <c r="I134" s="2"/>
+    </row>
+    <row r="135" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A135" s="157"/>
+      <c r="B135" s="164"/>
+      <c r="C135" s="159"/>
+      <c r="D135" s="160"/>
+      <c r="E135" s="161"/>
+      <c r="F135" s="162"/>
+      <c r="G135" s="161"/>
+      <c r="I135" s="2"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="165"/>
+      <c r="C136" s="36"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="39"/>
+      <c r="F136" s="86"/>
+      <c r="G136" s="87"/>
+      <c r="I136" s="2"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="165"/>
+      <c r="C137" s="36"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="39"/>
+      <c r="F137" s="86"/>
+      <c r="G137" s="87"/>
+      <c r="I137" s="2"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="165"/>
+      <c r="C138" s="36"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="39"/>
+      <c r="F138" s="86"/>
+      <c r="G138" s="87"/>
+      <c r="I138" s="2"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="165"/>
+      <c r="C139" s="36"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="39"/>
+      <c r="F139" s="86"/>
+      <c r="G139" s="87"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="165"/>
+      <c r="C140" s="36"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="39"/>
+      <c r="F140" s="86"/>
+      <c r="G140" s="87"/>
+      <c r="I140" s="2"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="165"/>
+      <c r="C141" s="36"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="39"/>
+      <c r="F141" s="86"/>
+      <c r="G141" s="87"/>
+      <c r="I141" s="2"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="165"/>
+      <c r="C142" s="36"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="39"/>
+      <c r="F142" s="86"/>
+      <c r="G142" s="87"/>
+      <c r="I142" s="2"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="165"/>
+      <c r="C143" s="36"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="39"/>
+      <c r="F143" s="86"/>
+      <c r="G143" s="87"/>
+      <c r="I143" s="2"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="165"/>
+      <c r="C144" s="36"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="39"/>
+      <c r="F144" s="86"/>
+      <c r="G144" s="87"/>
+      <c r="I144" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E114:G114"/>
-    <mergeCell ref="E116:G116"/>
+    <mergeCell ref="E131:G131"/>
+    <mergeCell ref="E133:G133"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
fin de viernes 23 AGOSTO -21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 1 " sheetId="1" r:id="rId1"/>
@@ -5593,8 +5593,8 @@
   </sheetPr>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6513,7 +6513,9 @@
       <c r="D25" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="195"/>
+      <c r="E25" s="195">
+        <v>551</v>
+      </c>
       <c r="F25" s="193"/>
       <c r="H25" s="30">
         <v>22</v>
@@ -6539,12 +6541,18 @@
       <c r="A26" s="55">
         <v>23</v>
       </c>
-      <c r="B26" s="194"/>
-      <c r="C26" s="177"/>
+      <c r="B26" s="194">
+        <v>44428</v>
+      </c>
+      <c r="C26" s="177">
+        <v>24621.96</v>
+      </c>
       <c r="D26" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="195"/>
+      <c r="E26" s="195">
+        <v>552</v>
+      </c>
       <c r="F26" s="193"/>
       <c r="H26" s="55">
         <v>23</v>
@@ -6570,8 +6578,12 @@
       <c r="A27" s="30">
         <v>24</v>
       </c>
-      <c r="B27" s="196"/>
-      <c r="C27" s="177"/>
+      <c r="B27" s="196">
+        <v>44434</v>
+      </c>
+      <c r="C27" s="177">
+        <v>23223.96</v>
+      </c>
       <c r="D27" s="178" t="s">
         <v>16</v>
       </c>
@@ -22228,7 +22240,7 @@
   </sheetPr>
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
@@ -27094,7 +27106,7 @@
         <v>44415</v>
       </c>
       <c r="B70" s="12">
-        <f t="shared" ref="B70:B126" si="2">B69+1</f>
+        <f t="shared" ref="B70:B125" si="2">B69+1</f>
         <v>2359</v>
       </c>
       <c r="C70" s="21"/>

</xml_diff>

<commit_message>
CORTE 7 DESEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 1 " sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="76">
   <si>
     <t xml:space="preserve">ABASTO 4 CARNES </t>
   </si>
@@ -2638,13 +2638,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>156</xdr:row>
       <xdr:rowOff>152402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2691,13 +2691,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>561977</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>156</xdr:row>
       <xdr:rowOff>123829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5593,8 +5593,8 @@
   </sheetPr>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6736,12 +6736,18 @@
       <c r="A31" s="30">
         <v>28</v>
       </c>
-      <c r="B31" s="176"/>
-      <c r="C31" s="177"/>
+      <c r="B31" s="176">
+        <v>44443</v>
+      </c>
+      <c r="C31" s="177">
+        <v>12416.82</v>
+      </c>
       <c r="D31" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="180"/>
+      <c r="E31" s="180">
+        <v>585</v>
+      </c>
       <c r="F31" s="199"/>
       <c r="H31" s="30">
         <v>28</v>
@@ -6766,8 +6772,12 @@
       <c r="A32" s="30">
         <v>29</v>
       </c>
-      <c r="B32" s="176"/>
-      <c r="C32" s="177"/>
+      <c r="B32" s="176">
+        <v>44445</v>
+      </c>
+      <c r="C32" s="177">
+        <v>12893.4</v>
+      </c>
       <c r="D32" s="178" t="s">
         <v>16</v>
       </c>
@@ -25288,13 +25298,13 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:Q144"/>
+  <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D105" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E121" sqref="E121"/>
+      <selection pane="bottomRight" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -25382,7 +25392,7 @@
         <v>9594</v>
       </c>
       <c r="H4" s="16">
-        <f t="shared" ref="H4:H126" si="0">E4-G4</f>
+        <f t="shared" ref="H4:H155" si="0">E4-G4</f>
         <v>0</v>
       </c>
       <c r="I4" s="2"/>
@@ -27142,7 +27152,7 @@
         <v>44415</v>
       </c>
       <c r="B70" s="12">
-        <f t="shared" ref="B70:B125" si="2">B69+1</f>
+        <f t="shared" ref="B70:B133" si="2">B69+1</f>
         <v>2359</v>
       </c>
       <c r="C70" s="21"/>
@@ -27300,11 +27310,15 @@
       <c r="E75" s="20">
         <v>1654</v>
       </c>
-      <c r="F75" s="49"/>
-      <c r="G75" s="27"/>
+      <c r="F75" s="49">
+        <v>44438</v>
+      </c>
+      <c r="G75" s="27">
+        <v>1654</v>
+      </c>
       <c r="H75" s="28">
         <f t="shared" si="0"/>
-        <v>1654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
@@ -27842,11 +27856,15 @@
       <c r="E96" s="27">
         <v>8452</v>
       </c>
-      <c r="F96" s="214"/>
-      <c r="G96" s="27"/>
+      <c r="F96" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G96" s="27">
+        <v>8452</v>
+      </c>
       <c r="H96" s="28">
         <f t="shared" si="0"/>
-        <v>8452</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -28176,11 +28194,15 @@
       <c r="E109" s="27">
         <v>3795</v>
       </c>
-      <c r="F109" s="214"/>
-      <c r="G109" s="27"/>
+      <c r="F109" s="214">
+        <v>44433</v>
+      </c>
+      <c r="G109" s="27">
+        <v>3795</v>
+      </c>
       <c r="H109" s="28">
         <f t="shared" si="0"/>
-        <v>3795</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -28198,11 +28220,15 @@
       <c r="E110" s="27">
         <v>2064</v>
       </c>
-      <c r="F110" s="214"/>
-      <c r="G110" s="27"/>
+      <c r="F110" s="214">
+        <v>44432</v>
+      </c>
+      <c r="G110" s="27">
+        <v>2064</v>
+      </c>
       <c r="H110" s="28">
         <f t="shared" si="0"/>
-        <v>2064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -28257,7 +28283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="157">
         <v>44429</v>
       </c>
@@ -28283,7 +28309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="157">
         <v>44429</v>
       </c>
@@ -28309,7 +28335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="157">
         <v>44429</v>
       </c>
@@ -28324,14 +28350,18 @@
       <c r="E115" s="27">
         <v>3407</v>
       </c>
-      <c r="F115" s="214"/>
-      <c r="G115" s="27"/>
+      <c r="F115" s="214">
+        <v>44434</v>
+      </c>
+      <c r="G115" s="27">
+        <v>3407</v>
+      </c>
       <c r="H115" s="28">
         <f t="shared" si="0"/>
-        <v>3407</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="157">
         <v>44429</v>
       </c>
@@ -28357,7 +28387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="157">
         <v>44431</v>
       </c>
@@ -28372,14 +28402,18 @@
       <c r="E117" s="27">
         <v>7791</v>
       </c>
-      <c r="F117" s="214"/>
-      <c r="G117" s="27"/>
+      <c r="F117" s="214">
+        <v>44432</v>
+      </c>
+      <c r="G117" s="27">
+        <v>7791</v>
+      </c>
       <c r="H117" s="28">
         <f t="shared" si="0"/>
-        <v>7791</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="157">
         <v>44431</v>
       </c>
@@ -28394,14 +28428,18 @@
       <c r="E118" s="27">
         <v>4024</v>
       </c>
-      <c r="F118" s="214"/>
-      <c r="G118" s="27"/>
+      <c r="F118" s="214">
+        <v>44434</v>
+      </c>
+      <c r="G118" s="27">
+        <v>4024</v>
+      </c>
       <c r="H118" s="28">
         <f t="shared" si="0"/>
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="157">
         <v>44431</v>
       </c>
@@ -28416,14 +28454,18 @@
       <c r="E119" s="27">
         <v>38827</v>
       </c>
-      <c r="F119" s="214"/>
-      <c r="G119" s="27"/>
+      <c r="F119" s="214">
+        <v>44433</v>
+      </c>
+      <c r="G119" s="27">
+        <v>38827</v>
+      </c>
       <c r="H119" s="28">
         <f t="shared" si="0"/>
-        <v>38827</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="157">
         <v>44431</v>
       </c>
@@ -28438,300 +28480,1054 @@
       <c r="E120" s="27">
         <v>8866</v>
       </c>
-      <c r="F120" s="214"/>
-      <c r="G120" s="27"/>
+      <c r="F120" s="214">
+        <v>44432</v>
+      </c>
+      <c r="G120" s="27">
+        <v>8866</v>
+      </c>
       <c r="H120" s="28">
         <f t="shared" si="0"/>
-        <v>8866</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="157"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="157">
+        <v>44432</v>
+      </c>
       <c r="B121" s="12">
         <f t="shared" si="2"/>
         <v>2410</v>
       </c>
       <c r="C121" s="213"/>
-      <c r="D121" s="45"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="214"/>
-      <c r="G121" s="27"/>
+      <c r="D121" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E121" s="27">
+        <v>310</v>
+      </c>
+      <c r="F121" s="214">
+        <v>44435</v>
+      </c>
+      <c r="G121" s="27">
+        <v>310</v>
+      </c>
       <c r="H121" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="157"/>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="157">
+        <v>44432</v>
+      </c>
       <c r="B122" s="12">
         <f t="shared" si="2"/>
         <v>2411</v>
       </c>
       <c r="C122" s="213"/>
-      <c r="D122" s="45"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="214"/>
-      <c r="G122" s="27"/>
+      <c r="D122" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E122" s="27">
+        <v>6608</v>
+      </c>
+      <c r="F122" s="214">
+        <v>44433</v>
+      </c>
+      <c r="G122" s="27">
+        <v>6608</v>
+      </c>
       <c r="H122" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="157"/>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="157">
+        <v>44432</v>
+      </c>
       <c r="B123" s="12">
         <f t="shared" si="2"/>
         <v>2412</v>
       </c>
       <c r="C123" s="213"/>
-      <c r="D123" s="45"/>
-      <c r="E123" s="27"/>
-      <c r="F123" s="214"/>
-      <c r="G123" s="27"/>
+      <c r="D123" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E123" s="27">
+        <v>1943</v>
+      </c>
+      <c r="F123" s="214">
+        <v>44435</v>
+      </c>
+      <c r="G123" s="27">
+        <v>1943</v>
+      </c>
       <c r="H123" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="157"/>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="157">
+        <v>44432</v>
+      </c>
       <c r="B124" s="12">
         <f t="shared" si="2"/>
         <v>2413</v>
       </c>
       <c r="C124" s="213"/>
-      <c r="D124" s="45"/>
-      <c r="E124" s="27"/>
-      <c r="F124" s="214"/>
-      <c r="G124" s="27"/>
+      <c r="D124" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E124" s="27">
+        <v>1023</v>
+      </c>
+      <c r="F124" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G124" s="27">
+        <v>1023</v>
+      </c>
       <c r="H124" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="157"/>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="157">
+        <v>44433</v>
+      </c>
       <c r="B125" s="12">
         <f t="shared" si="2"/>
         <v>2414</v>
       </c>
       <c r="C125" s="213"/>
-      <c r="D125" s="45"/>
-      <c r="E125" s="27"/>
-      <c r="F125" s="214"/>
-      <c r="G125" s="27"/>
+      <c r="D125" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E125" s="27">
+        <v>4471</v>
+      </c>
+      <c r="F125" s="214">
+        <v>44438</v>
+      </c>
+      <c r="G125" s="27">
+        <v>4471</v>
+      </c>
       <c r="H125" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="31"/>
-      <c r="B126" s="215"/>
-      <c r="C126" s="33"/>
-      <c r="D126" s="34"/>
-      <c r="E126" s="35">
-        <v>0</v>
-      </c>
-      <c r="F126" s="82"/>
-      <c r="G126" s="83"/>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="157">
+        <v>44433</v>
+      </c>
+      <c r="B126" s="12">
+        <f t="shared" si="2"/>
+        <v>2415</v>
+      </c>
+      <c r="C126" s="213"/>
+      <c r="D126" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E126" s="27">
+        <v>2001</v>
+      </c>
+      <c r="F126" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G126" s="27">
+        <v>2001</v>
+      </c>
       <c r="H126" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I126" s="2"/>
-    </row>
-    <row r="127" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="165"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="37">
-        <f>SUM(E4:E126)</f>
-        <v>571602</v>
-      </c>
-      <c r="F127" s="37"/>
-      <c r="G127" s="37">
-        <f>SUM(G4:G126)</f>
-        <v>492722</v>
-      </c>
-      <c r="H127" s="38">
-        <f>SUM(H4:H126)</f>
-        <v>78880</v>
-      </c>
-      <c r="I127" s="2"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B128" s="165"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="39"/>
-      <c r="F128" s="86"/>
-      <c r="G128" s="87"/>
-      <c r="H128" s="40"/>
-      <c r="I128" s="2"/>
-    </row>
-    <row r="129" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B129" s="165"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="41" t="s">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="157">
+        <v>44433</v>
+      </c>
+      <c r="B127" s="12">
+        <f t="shared" si="2"/>
+        <v>2416</v>
+      </c>
+      <c r="C127" s="213"/>
+      <c r="D127" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E127" s="27">
+        <v>35291</v>
+      </c>
+      <c r="F127" s="214">
+        <v>44435</v>
+      </c>
+      <c r="G127" s="27">
+        <v>35291</v>
+      </c>
+      <c r="H127" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="157">
+        <v>44433</v>
+      </c>
+      <c r="B128" s="12">
+        <f t="shared" si="2"/>
+        <v>2417</v>
+      </c>
+      <c r="C128" s="213"/>
+      <c r="D128" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E128" s="27">
+        <v>8748</v>
+      </c>
+      <c r="F128" s="214">
+        <v>44434</v>
+      </c>
+      <c r="G128" s="27">
+        <v>8748</v>
+      </c>
+      <c r="H128" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="157">
+        <v>44434</v>
+      </c>
+      <c r="B129" s="12">
+        <f t="shared" si="2"/>
+        <v>2418</v>
+      </c>
+      <c r="C129" s="213"/>
+      <c r="D129" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E129" s="27">
+        <v>369</v>
+      </c>
+      <c r="F129" s="214">
+        <v>44438</v>
+      </c>
+      <c r="G129" s="27">
+        <v>369</v>
+      </c>
+      <c r="H129" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="157">
+        <v>44434</v>
+      </c>
+      <c r="B130" s="12">
+        <f t="shared" si="2"/>
+        <v>2419</v>
+      </c>
+      <c r="C130" s="213"/>
+      <c r="D130" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="E130" s="27">
+        <v>3046</v>
+      </c>
+      <c r="F130" s="216"/>
+      <c r="G130" s="92"/>
+      <c r="H130" s="28">
+        <f t="shared" si="0"/>
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="157">
+        <v>44434</v>
+      </c>
+      <c r="B131" s="12">
+        <f t="shared" si="2"/>
+        <v>2420</v>
+      </c>
+      <c r="C131" s="213"/>
+      <c r="D131" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E131" s="27">
+        <v>1635</v>
+      </c>
+      <c r="F131" s="214">
+        <v>44435</v>
+      </c>
+      <c r="G131" s="27">
+        <v>1635</v>
+      </c>
+      <c r="H131" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="157">
+        <v>44435</v>
+      </c>
+      <c r="B132" s="12">
+        <f t="shared" si="2"/>
+        <v>2421</v>
+      </c>
+      <c r="C132" s="213"/>
+      <c r="D132" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E132" s="27">
+        <v>35266</v>
+      </c>
+      <c r="F132" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G132" s="27">
+        <v>35266</v>
+      </c>
+      <c r="H132" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="157">
+        <v>44435</v>
+      </c>
+      <c r="B133" s="12">
+        <f t="shared" si="2"/>
+        <v>2422</v>
+      </c>
+      <c r="C133" s="213"/>
+      <c r="D133" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E133" s="27">
+        <v>4197</v>
+      </c>
+      <c r="F133" s="214">
+        <v>44437</v>
+      </c>
+      <c r="G133" s="27">
+        <v>4197</v>
+      </c>
+      <c r="H133" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="157">
+        <v>44435</v>
+      </c>
+      <c r="B134" s="12">
+        <f t="shared" ref="B134:B152" si="3">B133+1</f>
+        <v>2423</v>
+      </c>
+      <c r="C134" s="213"/>
+      <c r="D134" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E134" s="27">
+        <v>1825</v>
+      </c>
+      <c r="F134" s="214">
+        <v>44438</v>
+      </c>
+      <c r="G134" s="27">
+        <v>1825</v>
+      </c>
+      <c r="H134" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="157">
+        <v>44435</v>
+      </c>
+      <c r="B135" s="12">
+        <f t="shared" si="3"/>
+        <v>2424</v>
+      </c>
+      <c r="C135" s="213"/>
+      <c r="D135" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E135" s="27">
+        <v>7017</v>
+      </c>
+      <c r="F135" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G135" s="27">
+        <v>7017</v>
+      </c>
+      <c r="H135" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="157">
+        <v>44435</v>
+      </c>
+      <c r="B136" s="12">
+        <f t="shared" si="3"/>
+        <v>2425</v>
+      </c>
+      <c r="C136" s="213"/>
+      <c r="D136" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E136" s="27">
+        <v>1905</v>
+      </c>
+      <c r="F136" s="214">
+        <v>44436</v>
+      </c>
+      <c r="G136" s="27">
+        <v>1905</v>
+      </c>
+      <c r="H136" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B137" s="12">
+        <f t="shared" si="3"/>
+        <v>2426</v>
+      </c>
+      <c r="C137" s="213"/>
+      <c r="D137" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E137" s="27">
+        <v>98</v>
+      </c>
+      <c r="F137" s="214">
+        <v>44439</v>
+      </c>
+      <c r="G137" s="27">
+        <v>98</v>
+      </c>
+      <c r="H137" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B138" s="12">
+        <f t="shared" si="3"/>
+        <v>2427</v>
+      </c>
+      <c r="C138" s="213"/>
+      <c r="D138" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E138" s="27">
+        <v>2096</v>
+      </c>
+      <c r="F138" s="214">
+        <v>44437</v>
+      </c>
+      <c r="G138" s="27">
+        <v>2096</v>
+      </c>
+      <c r="H138" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B139" s="12">
+        <f t="shared" si="3"/>
+        <v>2428</v>
+      </c>
+      <c r="C139" s="213"/>
+      <c r="D139" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E139" s="27">
+        <v>3038</v>
+      </c>
+      <c r="F139" s="214">
+        <v>44438</v>
+      </c>
+      <c r="G139" s="27">
+        <v>3038</v>
+      </c>
+      <c r="H139" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B140" s="12">
+        <f t="shared" si="3"/>
+        <v>2429</v>
+      </c>
+      <c r="C140" s="213"/>
+      <c r="D140" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E140" s="27">
+        <v>32973</v>
+      </c>
+      <c r="F140" s="214">
+        <v>44439</v>
+      </c>
+      <c r="G140" s="27">
+        <v>32973</v>
+      </c>
+      <c r="H140" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B141" s="12">
+        <f t="shared" si="3"/>
+        <v>2430</v>
+      </c>
+      <c r="C141" s="213"/>
+      <c r="D141" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E141" s="27">
+        <v>14008</v>
+      </c>
+      <c r="F141" s="214">
+        <v>44437</v>
+      </c>
+      <c r="G141" s="27">
+        <v>14008</v>
+      </c>
+      <c r="H141" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B142" s="12">
+        <f t="shared" si="3"/>
+        <v>2431</v>
+      </c>
+      <c r="C142" s="213"/>
+      <c r="D142" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E142" s="27">
+        <v>2103</v>
+      </c>
+      <c r="F142" s="214">
+        <v>44437</v>
+      </c>
+      <c r="G142" s="27">
+        <v>2103</v>
+      </c>
+      <c r="H142" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="157">
+        <v>44436</v>
+      </c>
+      <c r="B143" s="12">
+        <f t="shared" si="3"/>
+        <v>2432</v>
+      </c>
+      <c r="C143" s="213"/>
+      <c r="D143" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E143" s="27">
+        <v>0</v>
+      </c>
+      <c r="F143" s="214"/>
+      <c r="G143" s="27"/>
+      <c r="H143" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="157">
+        <v>44437</v>
+      </c>
+      <c r="B144" s="12">
+        <f t="shared" si="3"/>
+        <v>2433</v>
+      </c>
+      <c r="C144" s="213"/>
+      <c r="D144" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E144" s="27">
+        <v>1905</v>
+      </c>
+      <c r="F144" s="214">
+        <v>44439</v>
+      </c>
+      <c r="G144" s="27">
+        <v>1905</v>
+      </c>
+      <c r="H144" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="157">
+        <v>44437</v>
+      </c>
+      <c r="B145" s="12">
+        <f t="shared" si="3"/>
+        <v>2434</v>
+      </c>
+      <c r="C145" s="213"/>
+      <c r="D145" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E145" s="27">
+        <v>3786</v>
+      </c>
+      <c r="F145" s="216"/>
+      <c r="G145" s="92"/>
+      <c r="H145" s="28">
+        <f t="shared" si="0"/>
+        <v>3786</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="157">
+        <v>44437</v>
+      </c>
+      <c r="B146" s="12">
+        <f t="shared" si="3"/>
+        <v>2435</v>
+      </c>
+      <c r="C146" s="213"/>
+      <c r="D146" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="E146" s="27">
+        <v>4244</v>
+      </c>
+      <c r="F146" s="214">
+        <v>44438</v>
+      </c>
+      <c r="G146" s="27">
+        <v>4244</v>
+      </c>
+      <c r="H146" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="157">
+        <v>44438</v>
+      </c>
+      <c r="B147" s="12">
+        <f t="shared" si="3"/>
+        <v>2436</v>
+      </c>
+      <c r="C147" s="213"/>
+      <c r="D147" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E147" s="27">
+        <v>1933</v>
+      </c>
+      <c r="F147" s="216"/>
+      <c r="G147" s="92"/>
+      <c r="H147" s="28">
+        <f t="shared" si="0"/>
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="157">
+        <v>44438</v>
+      </c>
+      <c r="B148" s="12">
+        <f t="shared" si="3"/>
+        <v>2437</v>
+      </c>
+      <c r="C148" s="213"/>
+      <c r="D148" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E148" s="27">
+        <v>1109</v>
+      </c>
+      <c r="F148" s="214">
+        <v>44439</v>
+      </c>
+      <c r="G148" s="27">
+        <v>1109</v>
+      </c>
+      <c r="H148" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="157">
+        <v>44438</v>
+      </c>
+      <c r="B149" s="12">
+        <f t="shared" si="3"/>
+        <v>2438</v>
+      </c>
+      <c r="C149" s="213"/>
+      <c r="D149" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E149" s="27">
+        <v>1744</v>
+      </c>
+      <c r="F149" s="216"/>
+      <c r="G149" s="92"/>
+      <c r="H149" s="28">
+        <f t="shared" si="0"/>
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="157">
+        <v>44438</v>
+      </c>
+      <c r="B150" s="12">
+        <f t="shared" si="3"/>
+        <v>2439</v>
+      </c>
+      <c r="C150" s="213"/>
+      <c r="D150" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="E150" s="27">
+        <v>8827</v>
+      </c>
+      <c r="F150" s="214">
+        <v>44439</v>
+      </c>
+      <c r="G150" s="27">
+        <v>8827</v>
+      </c>
+      <c r="H150" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="157">
+        <v>44439</v>
+      </c>
+      <c r="B151" s="12">
+        <f t="shared" si="3"/>
+        <v>2440</v>
+      </c>
+      <c r="C151" s="213"/>
+      <c r="D151" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E151" s="27">
+        <v>60</v>
+      </c>
+      <c r="F151" s="216"/>
+      <c r="G151" s="92"/>
+      <c r="H151" s="28">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="157">
+        <v>44439</v>
+      </c>
+      <c r="B152" s="12">
+        <f t="shared" si="3"/>
+        <v>2441</v>
+      </c>
+      <c r="C152" s="213"/>
+      <c r="D152" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E152" s="27">
+        <v>1617</v>
+      </c>
+      <c r="F152" s="216"/>
+      <c r="G152" s="92"/>
+      <c r="H152" s="28">
+        <f t="shared" si="0"/>
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="157"/>
+      <c r="B153" s="12"/>
+      <c r="C153" s="213"/>
+      <c r="D153" s="45"/>
+      <c r="E153" s="27"/>
+      <c r="F153" s="214"/>
+      <c r="G153" s="27"/>
+      <c r="H153" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="157"/>
+      <c r="B154" s="12"/>
+      <c r="C154" s="213"/>
+      <c r="D154" s="45"/>
+      <c r="E154" s="27"/>
+      <c r="F154" s="214"/>
+      <c r="G154" s="27"/>
+      <c r="H154" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="31"/>
+      <c r="B155" s="215"/>
+      <c r="C155" s="33"/>
+      <c r="D155" s="34"/>
+      <c r="E155" s="35">
+        <v>0</v>
+      </c>
+      <c r="F155" s="82"/>
+      <c r="G155" s="83"/>
+      <c r="H155" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I155" s="2"/>
+    </row>
+    <row r="156" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="165"/>
+      <c r="C156" s="36"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="37">
+        <f>SUM(E4:E155)</f>
+        <v>766798</v>
+      </c>
+      <c r="F156" s="37"/>
+      <c r="G156" s="37">
+        <f>SUM(G4:G155)</f>
+        <v>754612</v>
+      </c>
+      <c r="H156" s="38">
+        <f>SUM(H4:H155)</f>
+        <v>12186</v>
+      </c>
+      <c r="I156" s="2"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B157" s="165"/>
+      <c r="C157" s="36"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="39"/>
+      <c r="F157" s="86"/>
+      <c r="G157" s="87"/>
+      <c r="H157" s="40"/>
+      <c r="I157" s="2"/>
+    </row>
+    <row r="158" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B158" s="165"/>
+      <c r="C158" s="36"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F129" s="86"/>
-      <c r="G129" s="88" t="s">
+      <c r="F158" s="86"/>
+      <c r="G158" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="H129" s="40"/>
-      <c r="I129" s="2"/>
-    </row>
-    <row r="130" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="165"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="41"/>
-      <c r="F130" s="86"/>
-      <c r="G130" s="88"/>
-      <c r="H130" s="40"/>
-      <c r="I130" s="2"/>
-    </row>
-    <row r="131" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B131" s="165"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="221">
-        <f>E127-G127</f>
-        <v>78880</v>
-      </c>
-      <c r="F131" s="222"/>
-      <c r="G131" s="223"/>
-      <c r="I131" s="2"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="165"/>
-      <c r="C132" s="36"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="39"/>
-      <c r="F132" s="86"/>
-      <c r="G132" s="87"/>
-      <c r="I132" s="2"/>
-    </row>
-    <row r="133" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B133" s="165"/>
-      <c r="C133" s="36"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="224" t="s">
+      <c r="H158" s="40"/>
+      <c r="I158" s="2"/>
+    </row>
+    <row r="159" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="165"/>
+      <c r="C159" s="36"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="41"/>
+      <c r="F159" s="86"/>
+      <c r="G159" s="88"/>
+      <c r="H159" s="40"/>
+      <c r="I159" s="2"/>
+    </row>
+    <row r="160" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B160" s="165"/>
+      <c r="C160" s="36"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="221">
+        <f>E156-G156</f>
+        <v>12186</v>
+      </c>
+      <c r="F160" s="222"/>
+      <c r="G160" s="223"/>
+      <c r="I160" s="2"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B161" s="165"/>
+      <c r="C161" s="36"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="39"/>
+      <c r="F161" s="86"/>
+      <c r="G161" s="87"/>
+      <c r="I161" s="2"/>
+    </row>
+    <row r="162" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B162" s="165"/>
+      <c r="C162" s="36"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="F133" s="224"/>
-      <c r="G133" s="224"/>
-      <c r="I133" s="2"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B134" s="165"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="39"/>
-      <c r="F134" s="86"/>
-      <c r="G134" s="87"/>
-      <c r="I134" s="2"/>
-    </row>
-    <row r="135" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A135" s="157"/>
-      <c r="B135" s="164"/>
-      <c r="C135" s="159"/>
-      <c r="D135" s="160"/>
-      <c r="E135" s="161"/>
-      <c r="F135" s="162"/>
-      <c r="G135" s="161"/>
-      <c r="I135" s="2"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B136" s="165"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="39"/>
-      <c r="F136" s="86"/>
-      <c r="G136" s="87"/>
-      <c r="I136" s="2"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B137" s="165"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="39"/>
-      <c r="F137" s="86"/>
-      <c r="G137" s="87"/>
-      <c r="I137" s="2"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B138" s="165"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="39"/>
-      <c r="F138" s="86"/>
-      <c r="G138" s="87"/>
-      <c r="I138" s="2"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B139" s="165"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="39"/>
-      <c r="F139" s="86"/>
-      <c r="G139" s="87"/>
-      <c r="I139" s="2"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B140" s="165"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="39"/>
-      <c r="F140" s="86"/>
-      <c r="G140" s="87"/>
-      <c r="I140" s="2"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B141" s="165"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="39"/>
-      <c r="F141" s="86"/>
-      <c r="G141" s="87"/>
-      <c r="I141" s="2"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B142" s="165"/>
-      <c r="C142" s="36"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="39"/>
-      <c r="F142" s="86"/>
-      <c r="G142" s="87"/>
-      <c r="I142" s="2"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B143" s="165"/>
-      <c r="C143" s="36"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="39"/>
-      <c r="F143" s="86"/>
-      <c r="G143" s="87"/>
-      <c r="I143" s="2"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B144" s="165"/>
-      <c r="C144" s="36"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="39"/>
-      <c r="F144" s="86"/>
-      <c r="G144" s="87"/>
-      <c r="I144" s="2"/>
+      <c r="F162" s="224"/>
+      <c r="G162" s="224"/>
+      <c r="I162" s="2"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B163" s="165"/>
+      <c r="C163" s="36"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="39"/>
+      <c r="F163" s="86"/>
+      <c r="G163" s="87"/>
+      <c r="I163" s="2"/>
+    </row>
+    <row r="164" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A164" s="157"/>
+      <c r="B164" s="164"/>
+      <c r="C164" s="159"/>
+      <c r="D164" s="160"/>
+      <c r="E164" s="161"/>
+      <c r="F164" s="162"/>
+      <c r="G164" s="161"/>
+      <c r="I164" s="2"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B165" s="165"/>
+      <c r="C165" s="36"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="39"/>
+      <c r="F165" s="86"/>
+      <c r="G165" s="87"/>
+      <c r="I165" s="2"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B166" s="165"/>
+      <c r="C166" s="36"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="39"/>
+      <c r="F166" s="86"/>
+      <c r="G166" s="87"/>
+      <c r="I166" s="2"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B167" s="165"/>
+      <c r="C167" s="36"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="39"/>
+      <c r="F167" s="86"/>
+      <c r="G167" s="87"/>
+      <c r="I167" s="2"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B168" s="165"/>
+      <c r="C168" s="36"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="39"/>
+      <c r="F168" s="86"/>
+      <c r="G168" s="87"/>
+      <c r="I168" s="2"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B169" s="165"/>
+      <c r="C169" s="36"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="39"/>
+      <c r="F169" s="86"/>
+      <c r="G169" s="87"/>
+      <c r="I169" s="2"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B170" s="165"/>
+      <c r="C170" s="36"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="39"/>
+      <c r="F170" s="86"/>
+      <c r="G170" s="87"/>
+      <c r="I170" s="2"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B171" s="165"/>
+      <c r="C171" s="36"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="39"/>
+      <c r="F171" s="86"/>
+      <c r="G171" s="87"/>
+      <c r="I171" s="2"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B172" s="165"/>
+      <c r="C172" s="36"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="39"/>
+      <c r="F172" s="86"/>
+      <c r="G172" s="87"/>
+      <c r="I172" s="2"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B173" s="165"/>
+      <c r="C173" s="36"/>
+      <c r="D173" s="2"/>
+      <c r="E173" s="39"/>
+      <c r="F173" s="86"/>
+      <c r="G173" s="87"/>
+      <c r="I173" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="E131:G131"/>
-    <mergeCell ref="E133:G133"/>
+    <mergeCell ref="E160:G160"/>
+    <mergeCell ref="E162:G162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 8 SEP 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -5594,7 +5594,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6748,7 +6748,9 @@
       <c r="E31" s="180">
         <v>585</v>
       </c>
-      <c r="F31" s="199"/>
+      <c r="F31" s="199">
+        <v>44447</v>
+      </c>
       <c r="H31" s="30">
         <v>28</v>
       </c>
@@ -6784,7 +6786,9 @@
       <c r="E32" s="180">
         <v>592</v>
       </c>
-      <c r="F32" s="199"/>
+      <c r="F32" s="199">
+        <v>44447</v>
+      </c>
       <c r="H32" s="30">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
FINAL 14 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -5594,7 +5594,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6824,7 +6824,9 @@
       <c r="E33" s="180">
         <v>594</v>
       </c>
-      <c r="F33" s="199"/>
+      <c r="F33" s="199">
+        <v>44452</v>
+      </c>
       <c r="H33" s="30">
         <v>30</v>
       </c>
@@ -6882,13 +6884,21 @@
       <c r="A35" s="30">
         <v>32</v>
       </c>
-      <c r="B35" s="176"/>
-      <c r="C35" s="177"/>
+      <c r="B35" s="176">
+        <v>44450</v>
+      </c>
+      <c r="C35" s="177">
+        <v>24289.26</v>
+      </c>
       <c r="D35" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="180"/>
-      <c r="F35" s="199"/>
+      <c r="E35" s="180">
+        <v>601</v>
+      </c>
+      <c r="F35" s="199">
+        <v>44453</v>
+      </c>
       <c r="H35" s="30">
         <v>32</v>
       </c>
@@ -6912,8 +6922,12 @@
       <c r="A36" s="30">
         <v>33</v>
       </c>
-      <c r="B36" s="176"/>
-      <c r="C36" s="177"/>
+      <c r="B36" s="176">
+        <v>44452</v>
+      </c>
+      <c r="C36" s="177">
+        <v>11810.5</v>
+      </c>
       <c r="D36" s="178" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
fin de 21 de Sept 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -5593,8 +5593,8 @@
   </sheetPr>
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6859,7 +6859,9 @@
       <c r="D34" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="180"/>
+      <c r="E34" s="180">
+        <v>609</v>
+      </c>
       <c r="F34" s="199"/>
       <c r="H34" s="30">
         <v>31</v>
@@ -6956,12 +6958,18 @@
       <c r="A37" s="30">
         <v>34</v>
       </c>
-      <c r="B37" s="176"/>
-      <c r="C37" s="177"/>
+      <c r="B37" s="176">
+        <v>44456</v>
+      </c>
+      <c r="C37" s="177">
+        <v>23874.19</v>
+      </c>
       <c r="D37" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="180"/>
+      <c r="E37" s="180">
+        <v>612</v>
+      </c>
       <c r="F37" s="199"/>
       <c r="H37" s="30">
         <v>34</v>

</xml_diff>

<commit_message>
CIERRE 23 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 08 AGOSTO  2021/CREDITOS  4 CARNES  AGOSTO      2021.xlsx
@@ -5594,7 +5594,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6862,7 +6862,9 @@
       <c r="E34" s="180">
         <v>609</v>
       </c>
-      <c r="F34" s="199"/>
+      <c r="F34" s="199">
+        <v>44461</v>
+      </c>
       <c r="H34" s="30">
         <v>31</v>
       </c>
@@ -6970,7 +6972,9 @@
       <c r="E37" s="180">
         <v>612</v>
       </c>
-      <c r="F37" s="199"/>
+      <c r="F37" s="199">
+        <v>44461</v>
+      </c>
       <c r="H37" s="30">
         <v>34</v>
       </c>
@@ -6994,12 +6998,18 @@
       <c r="A38" s="30">
         <v>35</v>
       </c>
-      <c r="B38" s="176"/>
-      <c r="C38" s="200"/>
+      <c r="B38" s="176">
+        <v>44460</v>
+      </c>
+      <c r="C38" s="200">
+        <v>20001.48</v>
+      </c>
       <c r="D38" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="201"/>
+      <c r="E38" s="201">
+        <v>617</v>
+      </c>
       <c r="F38" s="199"/>
       <c r="H38" s="30">
         <v>35</v>

</xml_diff>